<commit_message>
Fetches Erstelldatum from JIRA field Erstelldatum, Template formatted
</commit_message>
<xml_diff>
--- a/template/Template.xlsx
+++ b/template/Template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DE7C22-D25E-B744-90E3-6FBA3A3B2773}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B4D173-BE63-934A-9C3B-48FA79838A9E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,9 +11,6 @@
     <sheet name="Offene Punkte" sheetId="1" r:id="rId1"/>
     <sheet name="Projektrisiken" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Offene Punkte'!$A$6:$I$72</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Projektrisiken!$A$6:$J$143</definedName>
@@ -516,37 +513,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{C7CAC533-5731-724E-81FD-B2C775F1C1C1}"/>
   </cellStyles>
-  <dxfs count="66">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF339933"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <color auto="1"/>
@@ -564,246 +531,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF339933"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF339933"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF339933"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF339933"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF339933"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF339933"/>
         </patternFill>
       </fill>
     </dxf>
@@ -852,288 +579,6 @@
         <color rgb="FF9C0006"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF339933"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF339933"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF339933"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF339933"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF339933"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF339933"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF339933"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF339933"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
@@ -1159,12 +604,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1493,7 +932,7 @@
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1915,7 +1354,7 @@
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
       <c r="D7" s="20"/>
-      <c r="E7" s="36"/>
+      <c r="E7" s="31"/>
       <c r="F7" s="36"/>
       <c r="G7" s="33"/>
       <c r="H7" s="20"/>
@@ -1978,7 +1417,7 @@
       <c r="B8" s="20"/>
       <c r="C8" s="20"/>
       <c r="D8" s="20"/>
-      <c r="E8" s="36"/>
+      <c r="E8" s="31"/>
       <c r="F8" s="36"/>
       <c r="G8" s="34"/>
       <c r="H8" s="20"/>
@@ -2041,7 +1480,7 @@
       <c r="B9" s="20"/>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
-      <c r="E9" s="36"/>
+      <c r="E9" s="31"/>
       <c r="F9" s="36"/>
       <c r="G9" s="34"/>
       <c r="H9" s="20"/>
@@ -2104,7 +1543,7 @@
       <c r="B10" s="20"/>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
-      <c r="E10" s="36"/>
+      <c r="E10" s="31"/>
       <c r="F10" s="36"/>
       <c r="G10" s="34"/>
       <c r="H10" s="20"/>
@@ -2167,7 +1606,7 @@
       <c r="B11" s="20"/>
       <c r="C11" s="20"/>
       <c r="D11" s="20"/>
-      <c r="E11" s="36"/>
+      <c r="E11" s="31"/>
       <c r="F11" s="36"/>
       <c r="G11" s="32"/>
       <c r="H11" s="20"/>
@@ -2230,7 +1669,7 @@
       <c r="B12" s="20"/>
       <c r="C12" s="20"/>
       <c r="D12" s="20"/>
-      <c r="E12" s="36"/>
+      <c r="E12" s="31"/>
       <c r="F12" s="36"/>
       <c r="G12" s="35"/>
       <c r="H12" s="20"/>
@@ -2293,7 +1732,7 @@
       <c r="B13" s="20"/>
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>
-      <c r="E13" s="36"/>
+      <c r="E13" s="31"/>
       <c r="F13" s="36"/>
       <c r="G13" s="34"/>
       <c r="H13" s="20"/>
@@ -2356,7 +1795,7 @@
       <c r="B14" s="20"/>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
-      <c r="E14" s="36"/>
+      <c r="E14" s="31"/>
       <c r="F14" s="36"/>
       <c r="G14" s="34"/>
       <c r="H14" s="20"/>
@@ -2419,7 +1858,7 @@
       <c r="B15" s="20"/>
       <c r="C15" s="20"/>
       <c r="D15" s="21"/>
-      <c r="E15" s="36"/>
+      <c r="E15" s="31"/>
       <c r="F15" s="36"/>
       <c r="G15" s="34"/>
       <c r="H15" s="20"/>
@@ -2430,7 +1869,7 @@
       <c r="B16" s="20"/>
       <c r="C16" s="20"/>
       <c r="D16" s="20"/>
-      <c r="E16" s="36"/>
+      <c r="E16" s="31"/>
       <c r="F16" s="36"/>
       <c r="G16" s="34"/>
       <c r="H16" s="20"/>
@@ -2441,7 +1880,7 @@
       <c r="B17" s="20"/>
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
-      <c r="E17" s="36"/>
+      <c r="E17" s="31"/>
       <c r="F17" s="36"/>
       <c r="G17" s="34"/>
       <c r="H17" s="20"/>
@@ -2461,7 +1900,7 @@
       <c r="B18" s="20"/>
       <c r="C18" s="20"/>
       <c r="D18" s="20"/>
-      <c r="E18" s="36"/>
+      <c r="E18" s="31"/>
       <c r="F18" s="36"/>
       <c r="G18" s="34"/>
       <c r="H18" s="20"/>
@@ -2481,7 +1920,7 @@
       <c r="B19" s="20"/>
       <c r="C19" s="20"/>
       <c r="D19" s="20"/>
-      <c r="E19" s="36"/>
+      <c r="E19" s="31"/>
       <c r="F19" s="36"/>
       <c r="G19" s="34"/>
       <c r="H19" s="20"/>
@@ -2501,7 +1940,7 @@
       <c r="B20" s="20"/>
       <c r="C20" s="20"/>
       <c r="D20" s="20"/>
-      <c r="E20" s="36"/>
+      <c r="E20" s="31"/>
       <c r="F20" s="36"/>
       <c r="G20" s="34"/>
       <c r="H20" s="20"/>
@@ -2521,7 +1960,7 @@
       <c r="B21" s="20"/>
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
-      <c r="E21" s="36"/>
+      <c r="E21" s="31"/>
       <c r="F21" s="36"/>
       <c r="G21" s="34"/>
       <c r="H21" s="20"/>
@@ -2541,7 +1980,7 @@
       <c r="B22" s="20"/>
       <c r="C22" s="20"/>
       <c r="D22" s="30"/>
-      <c r="E22" s="21"/>
+      <c r="E22" s="31"/>
       <c r="F22" s="31"/>
       <c r="G22" s="34"/>
       <c r="H22" s="20"/>
@@ -2561,7 +2000,7 @@
       <c r="B23" s="20"/>
       <c r="C23" s="20"/>
       <c r="D23" s="20"/>
-      <c r="E23" s="36"/>
+      <c r="E23" s="31"/>
       <c r="F23" s="36"/>
       <c r="G23" s="34"/>
       <c r="H23" s="21"/>
@@ -2581,7 +2020,7 @@
       <c r="B24" s="30"/>
       <c r="C24" s="20"/>
       <c r="D24" s="20"/>
-      <c r="E24" s="36"/>
+      <c r="E24" s="31"/>
       <c r="F24" s="36"/>
       <c r="G24" s="33"/>
       <c r="H24" s="21"/>
@@ -2601,7 +2040,7 @@
       <c r="B25" s="30"/>
       <c r="C25" s="20"/>
       <c r="D25" s="20"/>
-      <c r="E25" s="36"/>
+      <c r="E25" s="31"/>
       <c r="F25" s="36"/>
       <c r="G25" s="34"/>
       <c r="H25" s="21"/>
@@ -2621,7 +2060,7 @@
       <c r="B26" s="30"/>
       <c r="C26" s="20"/>
       <c r="D26" s="20"/>
-      <c r="E26" s="36"/>
+      <c r="E26" s="31"/>
       <c r="F26" s="36"/>
       <c r="G26" s="34"/>
       <c r="H26" s="20"/>
@@ -2641,7 +2080,7 @@
       <c r="B27" s="30"/>
       <c r="C27" s="20"/>
       <c r="D27" s="20"/>
-      <c r="E27" s="36"/>
+      <c r="E27" s="31"/>
       <c r="F27" s="36"/>
       <c r="G27" s="34"/>
       <c r="H27" s="20"/>
@@ -2661,7 +2100,7 @@
       <c r="B28" s="30"/>
       <c r="C28" s="30"/>
       <c r="D28" s="30"/>
-      <c r="E28" s="36"/>
+      <c r="E28" s="31"/>
       <c r="F28" s="36"/>
       <c r="G28" s="35"/>
       <c r="H28" s="30"/>
@@ -2681,7 +2120,7 @@
       <c r="B29" s="20"/>
       <c r="C29" s="20"/>
       <c r="D29" s="20"/>
-      <c r="E29" s="21"/>
+      <c r="E29" s="31"/>
       <c r="F29" s="31"/>
       <c r="G29" s="34"/>
       <c r="H29" s="20"/>
@@ -2721,7 +2160,7 @@
       <c r="B31" s="30"/>
       <c r="C31" s="30"/>
       <c r="D31" s="30"/>
-      <c r="E31" s="36"/>
+      <c r="E31" s="31"/>
       <c r="F31" s="36"/>
       <c r="G31" s="35"/>
       <c r="H31" s="30"/>
@@ -2741,7 +2180,7 @@
       <c r="B32" s="30"/>
       <c r="C32" s="30"/>
       <c r="D32" s="30"/>
-      <c r="E32" s="36"/>
+      <c r="E32" s="31"/>
       <c r="F32" s="36"/>
       <c r="G32" s="35"/>
       <c r="H32" s="30"/>
@@ -2761,7 +2200,7 @@
       <c r="B33" s="30"/>
       <c r="C33" s="30"/>
       <c r="D33" s="30"/>
-      <c r="E33" s="36"/>
+      <c r="E33" s="31"/>
       <c r="F33" s="36"/>
       <c r="G33" s="35"/>
       <c r="H33" s="30"/>
@@ -2781,7 +2220,7 @@
       <c r="B34" s="20"/>
       <c r="C34" s="20"/>
       <c r="D34" s="30"/>
-      <c r="E34" s="21"/>
+      <c r="E34" s="31"/>
       <c r="F34" s="31"/>
       <c r="G34" s="35"/>
       <c r="H34" s="20"/>
@@ -2801,7 +2240,7 @@
       <c r="B35" s="20"/>
       <c r="C35" s="20"/>
       <c r="D35" s="20"/>
-      <c r="E35" s="36"/>
+      <c r="E35" s="31"/>
       <c r="F35" s="36"/>
       <c r="G35" s="35"/>
       <c r="H35" s="20"/>
@@ -2821,7 +2260,7 @@
       <c r="B36" s="30"/>
       <c r="C36" s="30"/>
       <c r="D36" s="30"/>
-      <c r="E36" s="36"/>
+      <c r="E36" s="31"/>
       <c r="F36" s="36"/>
       <c r="G36" s="35"/>
       <c r="H36" s="30"/>
@@ -2841,7 +2280,7 @@
       <c r="B37" s="20"/>
       <c r="C37" s="20"/>
       <c r="D37" s="20"/>
-      <c r="E37" s="21"/>
+      <c r="E37" s="31"/>
       <c r="F37" s="31"/>
       <c r="G37" s="35"/>
       <c r="H37" s="20"/>
@@ -2861,7 +2300,7 @@
       <c r="B38" s="30"/>
       <c r="C38" s="30"/>
       <c r="D38" s="30"/>
-      <c r="E38" s="36"/>
+      <c r="E38" s="31"/>
       <c r="F38" s="36"/>
       <c r="G38" s="30"/>
       <c r="H38" s="30"/>
@@ -2894,7 +2333,7 @@
       <c r="B41" s="30"/>
       <c r="C41" s="32"/>
       <c r="D41" s="30"/>
-      <c r="E41" s="36"/>
+      <c r="E41" s="31"/>
       <c r="F41" s="36"/>
       <c r="G41" s="34"/>
       <c r="H41" s="32"/>
@@ -2914,7 +2353,7 @@
       <c r="B42" s="30"/>
       <c r="C42" s="32"/>
       <c r="D42" s="30"/>
-      <c r="E42" s="36"/>
+      <c r="E42" s="31"/>
       <c r="F42" s="36"/>
       <c r="G42" s="34"/>
       <c r="H42" s="32"/>
@@ -2934,7 +2373,7 @@
       <c r="B43" s="30"/>
       <c r="C43" s="32"/>
       <c r="D43" s="30"/>
-      <c r="E43" s="36"/>
+      <c r="E43" s="31"/>
       <c r="F43" s="36"/>
       <c r="G43" s="30"/>
       <c r="H43" s="32"/>
@@ -2954,7 +2393,7 @@
       <c r="B44" s="30"/>
       <c r="C44" s="32"/>
       <c r="D44" s="32"/>
-      <c r="E44" s="36"/>
+      <c r="E44" s="31"/>
       <c r="F44" s="36"/>
       <c r="G44" s="30"/>
       <c r="H44" s="32"/>
@@ -2974,7 +2413,7 @@
       <c r="B45" s="30"/>
       <c r="C45" s="30"/>
       <c r="D45" s="30"/>
-      <c r="E45" s="36"/>
+      <c r="E45" s="31"/>
       <c r="F45" s="36"/>
       <c r="G45" s="30"/>
       <c r="H45" s="30"/>
@@ -2985,7 +2424,7 @@
       <c r="B46" s="20"/>
       <c r="C46" s="20"/>
       <c r="D46" s="20"/>
-      <c r="E46" s="36"/>
+      <c r="E46" s="31"/>
       <c r="F46" s="36"/>
       <c r="G46" s="20"/>
       <c r="H46" s="20"/>
@@ -2996,7 +2435,7 @@
       <c r="B47" s="20"/>
       <c r="C47" s="20"/>
       <c r="D47" s="20"/>
-      <c r="E47" s="36"/>
+      <c r="E47" s="31"/>
       <c r="F47" s="36"/>
       <c r="G47" s="20"/>
       <c r="H47" s="20"/>
@@ -3007,7 +2446,7 @@
       <c r="B48" s="20"/>
       <c r="C48" s="20"/>
       <c r="D48" s="20"/>
-      <c r="E48" s="36"/>
+      <c r="E48" s="31"/>
       <c r="F48" s="36"/>
       <c r="G48" s="20"/>
       <c r="H48" s="20"/>
@@ -3018,7 +2457,7 @@
       <c r="B49" s="20"/>
       <c r="C49" s="20"/>
       <c r="D49" s="20"/>
-      <c r="E49" s="36"/>
+      <c r="E49" s="31"/>
       <c r="F49" s="36"/>
       <c r="G49" s="20"/>
       <c r="H49" s="20"/>
@@ -3029,7 +2468,7 @@
       <c r="B50" s="20"/>
       <c r="C50" s="20"/>
       <c r="D50" s="20"/>
-      <c r="E50" s="36"/>
+      <c r="E50" s="31"/>
       <c r="F50" s="36"/>
       <c r="G50" s="20"/>
       <c r="H50" s="20"/>
@@ -3040,7 +2479,7 @@
       <c r="B51" s="20"/>
       <c r="C51" s="20"/>
       <c r="D51" s="20"/>
-      <c r="E51" s="36"/>
+      <c r="E51" s="31"/>
       <c r="F51" s="36"/>
       <c r="G51" s="30"/>
       <c r="H51" s="20"/>
@@ -3051,7 +2490,7 @@
       <c r="B52" s="20"/>
       <c r="C52" s="20"/>
       <c r="D52" s="20"/>
-      <c r="E52" s="21"/>
+      <c r="E52" s="31"/>
       <c r="F52" s="31"/>
       <c r="G52" s="20"/>
       <c r="H52" s="20"/>
@@ -3062,7 +2501,7 @@
       <c r="B53" s="20"/>
       <c r="C53" s="20"/>
       <c r="D53" s="20"/>
-      <c r="E53" s="21"/>
+      <c r="E53" s="31"/>
       <c r="F53" s="31"/>
       <c r="G53" s="20"/>
       <c r="H53" s="20"/>
@@ -3073,7 +2512,7 @@
       <c r="B54" s="30"/>
       <c r="C54" s="30"/>
       <c r="D54" s="30"/>
-      <c r="E54" s="36"/>
+      <c r="E54" s="31"/>
       <c r="F54" s="36"/>
       <c r="G54" s="30"/>
       <c r="H54" s="30"/>
@@ -3084,7 +2523,7 @@
       <c r="B55" s="30"/>
       <c r="C55" s="30"/>
       <c r="D55" s="30"/>
-      <c r="E55" s="36"/>
+      <c r="E55" s="31"/>
       <c r="F55" s="36"/>
       <c r="G55" s="30"/>
       <c r="H55" s="30"/>
@@ -3106,7 +2545,7 @@
       <c r="B57" s="30"/>
       <c r="C57" s="30"/>
       <c r="D57" s="30"/>
-      <c r="E57" s="36"/>
+      <c r="E57" s="31"/>
       <c r="F57" s="36"/>
       <c r="G57" s="30"/>
       <c r="H57" s="30"/>
@@ -3117,7 +2556,7 @@
       <c r="B58" s="20"/>
       <c r="C58" s="20"/>
       <c r="D58" s="20"/>
-      <c r="E58" s="21"/>
+      <c r="E58" s="31"/>
       <c r="F58" s="31"/>
       <c r="G58" s="20"/>
       <c r="H58" s="20"/>
@@ -3128,7 +2567,7 @@
       <c r="B59" s="30"/>
       <c r="C59" s="30"/>
       <c r="D59" s="20"/>
-      <c r="E59" s="36"/>
+      <c r="E59" s="31"/>
       <c r="F59" s="36"/>
       <c r="G59" s="34"/>
       <c r="H59" s="30"/>
@@ -3139,7 +2578,7 @@
       <c r="B60" s="30"/>
       <c r="C60" s="30"/>
       <c r="D60" s="30"/>
-      <c r="E60" s="36"/>
+      <c r="E60" s="31"/>
       <c r="F60" s="36"/>
       <c r="G60" s="30"/>
       <c r="H60" s="30"/>
@@ -3150,7 +2589,7 @@
       <c r="B61" s="20"/>
       <c r="C61" s="20"/>
       <c r="D61" s="20"/>
-      <c r="E61" s="36"/>
+      <c r="E61" s="31"/>
       <c r="F61" s="36"/>
       <c r="G61" s="30"/>
       <c r="H61" s="20"/>
@@ -3161,7 +2600,7 @@
       <c r="B62" s="30"/>
       <c r="C62" s="30"/>
       <c r="D62" s="30"/>
-      <c r="E62" s="36"/>
+      <c r="E62" s="31"/>
       <c r="F62" s="36"/>
       <c r="G62" s="30"/>
       <c r="H62" s="30"/>
@@ -3172,7 +2611,7 @@
       <c r="B63" s="30"/>
       <c r="C63" s="30"/>
       <c r="D63" s="30"/>
-      <c r="E63" s="36"/>
+      <c r="E63" s="31"/>
       <c r="F63" s="36"/>
       <c r="G63" s="30"/>
       <c r="H63" s="30"/>
@@ -3183,7 +2622,7 @@
       <c r="B64" s="30"/>
       <c r="C64" s="30"/>
       <c r="D64" s="30"/>
-      <c r="E64" s="36"/>
+      <c r="E64" s="31"/>
       <c r="F64" s="36"/>
       <c r="G64" s="30"/>
       <c r="H64" s="30"/>
@@ -3194,7 +2633,7 @@
       <c r="B65" s="30"/>
       <c r="C65" s="30"/>
       <c r="D65" s="30"/>
-      <c r="E65" s="36"/>
+      <c r="E65" s="31"/>
       <c r="F65" s="36"/>
       <c r="G65" s="30"/>
       <c r="H65" s="30"/>
@@ -3205,7 +2644,7 @@
       <c r="B66" s="30"/>
       <c r="C66" s="30"/>
       <c r="D66" s="30"/>
-      <c r="E66" s="36"/>
+      <c r="E66" s="31"/>
       <c r="F66" s="36"/>
       <c r="G66" s="30"/>
       <c r="H66" s="30"/>
@@ -3216,7 +2655,7 @@
       <c r="B67" s="30"/>
       <c r="C67" s="30"/>
       <c r="D67" s="30"/>
-      <c r="E67" s="36"/>
+      <c r="E67" s="31"/>
       <c r="F67" s="36"/>
       <c r="G67" s="30"/>
       <c r="H67" s="30"/>
@@ -3227,7 +2666,7 @@
       <c r="B68" s="30"/>
       <c r="C68" s="30"/>
       <c r="D68" s="30"/>
-      <c r="E68" s="36"/>
+      <c r="E68" s="31"/>
       <c r="F68" s="36"/>
       <c r="G68" s="30"/>
       <c r="H68" s="30"/>
@@ -3238,7 +2677,7 @@
       <c r="B69" s="30"/>
       <c r="C69" s="30"/>
       <c r="D69" s="30"/>
-      <c r="E69" s="36"/>
+      <c r="E69" s="31"/>
       <c r="F69" s="36"/>
       <c r="G69" s="30"/>
       <c r="H69" s="30"/>
@@ -3249,7 +2688,7 @@
       <c r="B70" s="20"/>
       <c r="C70" s="20"/>
       <c r="D70" s="20"/>
-      <c r="E70" s="36"/>
+      <c r="E70" s="31"/>
       <c r="F70" s="36"/>
       <c r="G70" s="20"/>
       <c r="H70" s="20"/>
@@ -3260,7 +2699,7 @@
       <c r="B71" s="20"/>
       <c r="C71" s="20"/>
       <c r="D71" s="20"/>
-      <c r="E71" s="36"/>
+      <c r="E71" s="31"/>
       <c r="F71" s="36"/>
       <c r="G71" s="20"/>
       <c r="H71" s="20"/>
@@ -3271,7 +2710,7 @@
       <c r="B72" s="20"/>
       <c r="C72" s="20"/>
       <c r="D72" s="20"/>
-      <c r="E72" s="36"/>
+      <c r="E72" s="31"/>
       <c r="F72" s="36"/>
       <c r="G72" s="20"/>
       <c r="H72" s="20"/>
@@ -3282,7 +2721,7 @@
       <c r="B73" s="30"/>
       <c r="C73" s="30"/>
       <c r="D73" s="30"/>
-      <c r="E73" s="36"/>
+      <c r="E73" s="31"/>
       <c r="F73" s="36"/>
       <c r="G73" s="30"/>
       <c r="H73" s="30"/>
@@ -3293,7 +2732,7 @@
       <c r="B74" s="30"/>
       <c r="C74" s="30"/>
       <c r="D74" s="30"/>
-      <c r="E74" s="36"/>
+      <c r="E74" s="31"/>
       <c r="F74" s="36"/>
       <c r="G74" s="30"/>
       <c r="H74" s="30"/>
@@ -3304,7 +2743,7 @@
       <c r="B75" s="30"/>
       <c r="C75" s="30"/>
       <c r="D75" s="30"/>
-      <c r="E75" s="36"/>
+      <c r="E75" s="31"/>
       <c r="F75" s="36"/>
       <c r="G75" s="30"/>
       <c r="H75" s="30"/>
@@ -3315,7 +2754,7 @@
       <c r="B76" s="30"/>
       <c r="C76" s="30"/>
       <c r="D76" s="30"/>
-      <c r="E76" s="36"/>
+      <c r="E76" s="31"/>
       <c r="F76" s="36"/>
       <c r="G76" s="30"/>
       <c r="H76" s="30"/>
@@ -3326,7 +2765,7 @@
       <c r="B77" s="30"/>
       <c r="C77" s="30"/>
       <c r="D77" s="30"/>
-      <c r="E77" s="36"/>
+      <c r="E77" s="31"/>
       <c r="F77" s="36"/>
       <c r="G77" s="30"/>
       <c r="H77" s="30"/>
@@ -3337,7 +2776,7 @@
       <c r="B78" s="20"/>
       <c r="C78" s="20"/>
       <c r="D78" s="20"/>
-      <c r="E78" s="36"/>
+      <c r="E78" s="31"/>
       <c r="F78" s="36"/>
       <c r="G78" s="20"/>
       <c r="H78" s="20"/>
@@ -3348,7 +2787,7 @@
       <c r="B79" s="20"/>
       <c r="C79" s="20"/>
       <c r="D79" s="20"/>
-      <c r="E79" s="36"/>
+      <c r="E79" s="31"/>
       <c r="F79" s="36"/>
       <c r="G79" s="20"/>
       <c r="H79" s="20"/>
@@ -3359,7 +2798,7 @@
       <c r="B80" s="20"/>
       <c r="C80" s="20"/>
       <c r="D80" s="20"/>
-      <c r="E80" s="36"/>
+      <c r="E80" s="31"/>
       <c r="F80" s="36"/>
       <c r="G80" s="20"/>
       <c r="H80" s="20"/>
@@ -3370,7 +2809,7 @@
       <c r="B81" s="20"/>
       <c r="C81" s="20"/>
       <c r="D81" s="20"/>
-      <c r="E81" s="36"/>
+      <c r="E81" s="31"/>
       <c r="F81" s="36"/>
       <c r="G81" s="20"/>
       <c r="H81" s="20"/>
@@ -3381,7 +2820,7 @@
       <c r="B82" s="20"/>
       <c r="C82" s="20"/>
       <c r="D82" s="20"/>
-      <c r="E82" s="36"/>
+      <c r="E82" s="31"/>
       <c r="F82" s="36"/>
       <c r="G82" s="20"/>
       <c r="H82" s="20"/>
@@ -3392,7 +2831,7 @@
       <c r="B83" s="20"/>
       <c r="C83" s="20"/>
       <c r="D83" s="20"/>
-      <c r="E83" s="36"/>
+      <c r="E83" s="31"/>
       <c r="F83" s="36"/>
       <c r="G83" s="20"/>
       <c r="H83" s="20"/>
@@ -3403,7 +2842,7 @@
       <c r="B84" s="20"/>
       <c r="C84" s="20"/>
       <c r="D84" s="20"/>
-      <c r="E84" s="36"/>
+      <c r="E84" s="31"/>
       <c r="F84" s="36"/>
       <c r="G84" s="20"/>
       <c r="H84" s="20"/>
@@ -3414,7 +2853,7 @@
       <c r="B85" s="20"/>
       <c r="C85" s="20"/>
       <c r="D85" s="20"/>
-      <c r="E85" s="36"/>
+      <c r="E85" s="31"/>
       <c r="F85" s="36"/>
       <c r="G85" s="20"/>
       <c r="H85" s="20"/>
@@ -3425,7 +2864,7 @@
       <c r="B86" s="20"/>
       <c r="C86" s="20"/>
       <c r="D86" s="20"/>
-      <c r="E86" s="36"/>
+      <c r="E86" s="31"/>
       <c r="F86" s="36"/>
       <c r="G86" s="20"/>
       <c r="H86" s="20"/>
@@ -3436,7 +2875,7 @@
       <c r="B87" s="20"/>
       <c r="C87" s="20"/>
       <c r="D87" s="20"/>
-      <c r="E87" s="36"/>
+      <c r="E87" s="31"/>
       <c r="F87" s="36"/>
       <c r="G87" s="20"/>
       <c r="H87" s="20"/>
@@ -3447,7 +2886,7 @@
       <c r="B88" s="20"/>
       <c r="C88" s="20"/>
       <c r="D88" s="20"/>
-      <c r="E88" s="36"/>
+      <c r="E88" s="31"/>
       <c r="F88" s="36"/>
       <c r="G88" s="20"/>
       <c r="H88" s="20"/>
@@ -3458,7 +2897,7 @@
       <c r="B89" s="20"/>
       <c r="C89" s="20"/>
       <c r="D89" s="20"/>
-      <c r="E89" s="36"/>
+      <c r="E89" s="31"/>
       <c r="F89" s="36"/>
       <c r="G89" s="20"/>
       <c r="H89" s="20"/>
@@ -3469,7 +2908,7 @@
       <c r="B90" s="20"/>
       <c r="C90" s="20"/>
       <c r="D90" s="20"/>
-      <c r="E90" s="36"/>
+      <c r="E90" s="31"/>
       <c r="F90" s="36"/>
       <c r="G90" s="20"/>
       <c r="H90" s="20"/>
@@ -3480,7 +2919,7 @@
       <c r="B91" s="20"/>
       <c r="C91" s="20"/>
       <c r="D91" s="20"/>
-      <c r="E91" s="36"/>
+      <c r="E91" s="31"/>
       <c r="F91" s="36"/>
       <c r="G91" s="20"/>
       <c r="H91" s="20"/>
@@ -3491,7 +2930,7 @@
       <c r="B92" s="20"/>
       <c r="C92" s="20"/>
       <c r="D92" s="20"/>
-      <c r="E92" s="36"/>
+      <c r="E92" s="31"/>
       <c r="F92" s="36"/>
       <c r="G92" s="20"/>
       <c r="H92" s="20"/>
@@ -3502,7 +2941,7 @@
       <c r="B93" s="20"/>
       <c r="C93" s="20"/>
       <c r="D93" s="20"/>
-      <c r="E93" s="36"/>
+      <c r="E93" s="31"/>
       <c r="F93" s="36"/>
       <c r="G93" s="20"/>
       <c r="H93" s="20"/>
@@ -3513,7 +2952,7 @@
       <c r="B94" s="20"/>
       <c r="C94" s="20"/>
       <c r="D94" s="20"/>
-      <c r="E94" s="36"/>
+      <c r="E94" s="31"/>
       <c r="F94" s="36"/>
       <c r="G94" s="20"/>
       <c r="H94" s="20"/>
@@ -3524,7 +2963,7 @@
       <c r="B95" s="20"/>
       <c r="C95" s="20"/>
       <c r="D95" s="20"/>
-      <c r="E95" s="36"/>
+      <c r="E95" s="31"/>
       <c r="F95" s="36"/>
       <c r="G95" s="20"/>
       <c r="H95" s="20"/>
@@ -3535,7 +2974,7 @@
       <c r="B96" s="20"/>
       <c r="C96" s="20"/>
       <c r="D96" s="20"/>
-      <c r="E96" s="36"/>
+      <c r="E96" s="31"/>
       <c r="F96" s="36"/>
       <c r="G96" s="20"/>
       <c r="H96" s="20"/>
@@ -3546,7 +2985,7 @@
       <c r="B97" s="20"/>
       <c r="C97" s="20"/>
       <c r="D97" s="20"/>
-      <c r="E97" s="36"/>
+      <c r="E97" s="31"/>
       <c r="F97" s="36"/>
       <c r="G97" s="20"/>
       <c r="H97" s="20"/>
@@ -3557,7 +2996,7 @@
       <c r="B98" s="20"/>
       <c r="C98" s="20"/>
       <c r="D98" s="20"/>
-      <c r="E98" s="36"/>
+      <c r="E98" s="31"/>
       <c r="F98" s="36"/>
       <c r="G98" s="20"/>
       <c r="H98" s="20"/>
@@ -3568,7 +3007,7 @@
       <c r="B99" s="20"/>
       <c r="C99" s="20"/>
       <c r="D99" s="20"/>
-      <c r="E99" s="36"/>
+      <c r="E99" s="31"/>
       <c r="F99" s="36"/>
       <c r="G99" s="20"/>
       <c r="H99" s="20"/>
@@ -3579,7 +3018,7 @@
       <c r="B100" s="20"/>
       <c r="C100" s="20"/>
       <c r="D100" s="20"/>
-      <c r="E100" s="36"/>
+      <c r="E100" s="31"/>
       <c r="F100" s="36"/>
       <c r="G100" s="20"/>
       <c r="H100" s="20"/>
@@ -3590,7 +3029,7 @@
       <c r="B101" s="20"/>
       <c r="C101" s="20"/>
       <c r="D101" s="20"/>
-      <c r="E101" s="36"/>
+      <c r="E101" s="31"/>
       <c r="F101" s="36"/>
       <c r="G101" s="20"/>
       <c r="H101" s="20"/>
@@ -3601,7 +3040,7 @@
       <c r="B102" s="30"/>
       <c r="C102" s="30"/>
       <c r="D102" s="30"/>
-      <c r="E102" s="36"/>
+      <c r="E102" s="31"/>
       <c r="F102" s="36"/>
       <c r="G102" s="30"/>
       <c r="H102" s="30"/>
@@ -3612,7 +3051,7 @@
       <c r="B103" s="30"/>
       <c r="C103" s="30"/>
       <c r="D103" s="30"/>
-      <c r="E103" s="36"/>
+      <c r="E103" s="31"/>
       <c r="F103" s="36"/>
       <c r="G103" s="30"/>
       <c r="H103" s="30"/>
@@ -3623,7 +3062,7 @@
       <c r="B104" s="30"/>
       <c r="C104" s="30"/>
       <c r="D104" s="30"/>
-      <c r="E104" s="36"/>
+      <c r="E104" s="31"/>
       <c r="F104" s="36"/>
       <c r="G104" s="30"/>
       <c r="H104" s="30"/>
@@ -3634,7 +3073,7 @@
       <c r="B105" s="30"/>
       <c r="C105" s="30"/>
       <c r="D105" s="30"/>
-      <c r="E105" s="36"/>
+      <c r="E105" s="31"/>
       <c r="F105" s="36"/>
       <c r="G105" s="30"/>
       <c r="H105" s="30"/>
@@ -3645,7 +3084,7 @@
       <c r="B106" s="30"/>
       <c r="C106" s="30"/>
       <c r="D106" s="30"/>
-      <c r="E106" s="36"/>
+      <c r="E106" s="31"/>
       <c r="F106" s="36"/>
       <c r="G106" s="30"/>
       <c r="H106" s="30"/>
@@ -3656,7 +3095,7 @@
       <c r="B107" s="30"/>
       <c r="C107" s="30"/>
       <c r="D107" s="30"/>
-      <c r="E107" s="36"/>
+      <c r="E107" s="31"/>
       <c r="F107" s="36"/>
       <c r="G107" s="30"/>
       <c r="H107" s="30"/>
@@ -3667,7 +3106,7 @@
       <c r="B108" s="30"/>
       <c r="C108" s="30"/>
       <c r="D108" s="30"/>
-      <c r="E108" s="36"/>
+      <c r="E108" s="31"/>
       <c r="F108" s="36"/>
       <c r="G108" s="30"/>
       <c r="H108" s="30"/>
@@ -3678,7 +3117,7 @@
       <c r="B109" s="30"/>
       <c r="C109" s="30"/>
       <c r="D109" s="30"/>
-      <c r="E109" s="36"/>
+      <c r="E109" s="31"/>
       <c r="F109" s="36"/>
       <c r="G109" s="30"/>
       <c r="H109" s="30"/>
@@ -3689,7 +3128,7 @@
       <c r="B110" s="30"/>
       <c r="C110" s="30"/>
       <c r="D110" s="30"/>
-      <c r="E110" s="36"/>
+      <c r="E110" s="31"/>
       <c r="F110" s="36"/>
       <c r="G110" s="30"/>
       <c r="H110" s="30"/>
@@ -3700,7 +3139,7 @@
       <c r="B111" s="30"/>
       <c r="C111" s="30"/>
       <c r="D111" s="30"/>
-      <c r="E111" s="36"/>
+      <c r="E111" s="31"/>
       <c r="F111" s="36"/>
       <c r="G111" s="30"/>
       <c r="H111" s="30"/>
@@ -3711,7 +3150,7 @@
       <c r="B112" s="30"/>
       <c r="C112" s="30"/>
       <c r="D112" s="30"/>
-      <c r="E112" s="36"/>
+      <c r="E112" s="31"/>
       <c r="F112" s="36"/>
       <c r="G112" s="30"/>
       <c r="H112" s="30"/>
@@ -3722,7 +3161,7 @@
       <c r="B113" s="30"/>
       <c r="C113" s="30"/>
       <c r="D113" s="30"/>
-      <c r="E113" s="36"/>
+      <c r="E113" s="31"/>
       <c r="F113" s="36"/>
       <c r="G113" s="30"/>
       <c r="H113" s="30"/>
@@ -3733,7 +3172,7 @@
       <c r="B114" s="30"/>
       <c r="C114" s="30"/>
       <c r="D114" s="30"/>
-      <c r="E114" s="36"/>
+      <c r="E114" s="31"/>
       <c r="F114" s="36"/>
       <c r="G114" s="30"/>
       <c r="H114" s="30"/>
@@ -3744,7 +3183,7 @@
       <c r="B115" s="30"/>
       <c r="C115" s="30"/>
       <c r="D115" s="30"/>
-      <c r="E115" s="36"/>
+      <c r="E115" s="31"/>
       <c r="F115" s="36"/>
       <c r="G115" s="30"/>
       <c r="H115" s="30"/>
@@ -3755,7 +3194,7 @@
       <c r="B116" s="30"/>
       <c r="C116" s="30"/>
       <c r="D116" s="30"/>
-      <c r="E116" s="36"/>
+      <c r="E116" s="31"/>
       <c r="F116" s="36"/>
       <c r="G116" s="30"/>
       <c r="H116" s="30"/>
@@ -3766,7 +3205,7 @@
       <c r="B117" s="30"/>
       <c r="C117" s="30"/>
       <c r="D117" s="30"/>
-      <c r="E117" s="36"/>
+      <c r="E117" s="31"/>
       <c r="F117" s="36"/>
       <c r="G117" s="30"/>
       <c r="H117" s="30"/>
@@ -3777,7 +3216,7 @@
       <c r="B118" s="30"/>
       <c r="C118" s="30"/>
       <c r="D118" s="30"/>
-      <c r="E118" s="36"/>
+      <c r="E118" s="31"/>
       <c r="F118" s="36"/>
       <c r="G118" s="30"/>
       <c r="H118" s="30"/>
@@ -3788,7 +3227,7 @@
       <c r="B119" s="30"/>
       <c r="C119" s="30"/>
       <c r="D119" s="30"/>
-      <c r="E119" s="36"/>
+      <c r="E119" s="31"/>
       <c r="F119" s="36"/>
       <c r="G119" s="30"/>
       <c r="H119" s="30"/>
@@ -3799,7 +3238,7 @@
       <c r="B120" s="30"/>
       <c r="C120" s="30"/>
       <c r="D120" s="30"/>
-      <c r="E120" s="36"/>
+      <c r="E120" s="31"/>
       <c r="F120" s="36"/>
       <c r="G120" s="30"/>
       <c r="H120" s="30"/>
@@ -3810,7 +3249,7 @@
       <c r="B121" s="30"/>
       <c r="C121" s="30"/>
       <c r="D121" s="30"/>
-      <c r="E121" s="36"/>
+      <c r="E121" s="31"/>
       <c r="F121" s="36"/>
       <c r="G121" s="30"/>
       <c r="H121" s="30"/>
@@ -3821,7 +3260,7 @@
       <c r="B122" s="30"/>
       <c r="C122" s="30"/>
       <c r="D122" s="30"/>
-      <c r="E122" s="36"/>
+      <c r="E122" s="31"/>
       <c r="F122" s="36"/>
       <c r="G122" s="30"/>
       <c r="H122" s="30"/>
@@ -3832,7 +3271,7 @@
       <c r="B123" s="30"/>
       <c r="C123" s="30"/>
       <c r="D123" s="30"/>
-      <c r="E123" s="36"/>
+      <c r="E123" s="31"/>
       <c r="F123" s="36"/>
       <c r="G123" s="30"/>
       <c r="H123" s="30"/>
@@ -3843,7 +3282,7 @@
       <c r="B124" s="30"/>
       <c r="C124" s="30"/>
       <c r="D124" s="30"/>
-      <c r="E124" s="36"/>
+      <c r="E124" s="31"/>
       <c r="F124" s="36"/>
       <c r="G124" s="30"/>
       <c r="H124" s="30"/>
@@ -3854,7 +3293,7 @@
       <c r="B125" s="30"/>
       <c r="C125" s="30"/>
       <c r="D125" s="30"/>
-      <c r="E125" s="36"/>
+      <c r="E125" s="31"/>
       <c r="F125" s="36"/>
       <c r="G125" s="30"/>
       <c r="H125" s="30"/>
@@ -3865,7 +3304,7 @@
       <c r="B126" s="30"/>
       <c r="C126" s="30"/>
       <c r="D126" s="30"/>
-      <c r="E126" s="36"/>
+      <c r="E126" s="31"/>
       <c r="F126" s="36"/>
       <c r="G126" s="30"/>
       <c r="H126" s="30"/>
@@ -3876,7 +3315,7 @@
       <c r="B127" s="30"/>
       <c r="C127" s="30"/>
       <c r="D127" s="30"/>
-      <c r="E127" s="36"/>
+      <c r="E127" s="31"/>
       <c r="F127" s="36"/>
       <c r="G127" s="30"/>
       <c r="H127" s="30"/>
@@ -3887,7 +3326,7 @@
       <c r="B128" s="30"/>
       <c r="C128" s="30"/>
       <c r="D128" s="30"/>
-      <c r="E128" s="36"/>
+      <c r="E128" s="31"/>
       <c r="F128" s="36"/>
       <c r="G128" s="30"/>
       <c r="H128" s="30"/>
@@ -3898,7 +3337,7 @@
       <c r="B129" s="30"/>
       <c r="C129" s="30"/>
       <c r="D129" s="30"/>
-      <c r="E129" s="36"/>
+      <c r="E129" s="31"/>
       <c r="F129" s="36"/>
       <c r="G129" s="30"/>
       <c r="H129" s="30"/>
@@ -3909,7 +3348,7 @@
       <c r="B130" s="30"/>
       <c r="C130" s="30"/>
       <c r="D130" s="30"/>
-      <c r="E130" s="36"/>
+      <c r="E130" s="31"/>
       <c r="F130" s="36"/>
       <c r="G130" s="30"/>
       <c r="H130" s="30"/>
@@ -3920,7 +3359,7 @@
       <c r="B131" s="30"/>
       <c r="C131" s="30"/>
       <c r="D131" s="30"/>
-      <c r="E131" s="36"/>
+      <c r="E131" s="31"/>
       <c r="F131" s="36"/>
       <c r="G131" s="30"/>
       <c r="H131" s="30"/>
@@ -3931,7 +3370,7 @@
       <c r="B132" s="30"/>
       <c r="C132" s="30"/>
       <c r="D132" s="30"/>
-      <c r="E132" s="36"/>
+      <c r="E132" s="31"/>
       <c r="F132" s="36"/>
       <c r="G132" s="30"/>
       <c r="H132" s="30"/>
@@ -3942,7 +3381,7 @@
       <c r="B133" s="30"/>
       <c r="C133" s="30"/>
       <c r="D133" s="30"/>
-      <c r="E133" s="36"/>
+      <c r="E133" s="31"/>
       <c r="F133" s="36"/>
       <c r="G133" s="30"/>
       <c r="H133" s="30"/>
@@ -3953,7 +3392,7 @@
       <c r="B134" s="30"/>
       <c r="C134" s="30"/>
       <c r="D134" s="30"/>
-      <c r="E134" s="36"/>
+      <c r="E134" s="31"/>
       <c r="F134" s="36"/>
       <c r="G134" s="30"/>
       <c r="H134" s="30"/>
@@ -3964,7 +3403,7 @@
       <c r="B135" s="30"/>
       <c r="C135" s="30"/>
       <c r="D135" s="30"/>
-      <c r="E135" s="36"/>
+      <c r="E135" s="31"/>
       <c r="F135" s="36"/>
       <c r="G135" s="30"/>
       <c r="H135" s="30"/>
@@ -3975,7 +3414,7 @@
       <c r="B136" s="30"/>
       <c r="C136" s="30"/>
       <c r="D136" s="30"/>
-      <c r="E136" s="36"/>
+      <c r="E136" s="31"/>
       <c r="F136" s="36"/>
       <c r="G136" s="30"/>
       <c r="H136" s="30"/>
@@ -3986,7 +3425,7 @@
       <c r="B137" s="30"/>
       <c r="C137" s="30"/>
       <c r="D137" s="30"/>
-      <c r="E137" s="36"/>
+      <c r="E137" s="31"/>
       <c r="F137" s="36"/>
       <c r="G137" s="30"/>
       <c r="H137" s="30"/>
@@ -3997,7 +3436,7 @@
       <c r="B138" s="30"/>
       <c r="C138" s="30"/>
       <c r="D138" s="30"/>
-      <c r="E138" s="36"/>
+      <c r="E138" s="31"/>
       <c r="F138" s="36"/>
       <c r="G138" s="30"/>
       <c r="H138" s="30"/>
@@ -4008,7 +3447,7 @@
       <c r="B139" s="30"/>
       <c r="C139" s="30"/>
       <c r="D139" s="30"/>
-      <c r="E139" s="36"/>
+      <c r="E139" s="31"/>
       <c r="F139" s="36"/>
       <c r="G139" s="30"/>
       <c r="H139" s="30"/>
@@ -4019,7 +3458,7 @@
       <c r="B140" s="30"/>
       <c r="C140" s="30"/>
       <c r="D140" s="30"/>
-      <c r="E140" s="36"/>
+      <c r="E140" s="31"/>
       <c r="F140" s="36"/>
       <c r="G140" s="30"/>
       <c r="H140" s="30"/>
@@ -4030,7 +3469,7 @@
       <c r="B141" s="30"/>
       <c r="C141" s="30"/>
       <c r="D141" s="30"/>
-      <c r="E141" s="36"/>
+      <c r="E141" s="31"/>
       <c r="F141" s="36"/>
       <c r="G141" s="30"/>
       <c r="H141" s="30"/>
@@ -4041,7 +3480,7 @@
       <c r="B142" s="30"/>
       <c r="C142" s="30"/>
       <c r="D142" s="30"/>
-      <c r="E142" s="36"/>
+      <c r="E142" s="31"/>
       <c r="F142" s="36"/>
       <c r="G142" s="30"/>
       <c r="H142" s="30"/>
@@ -4052,7 +3491,7 @@
       <c r="B143" s="30"/>
       <c r="C143" s="30"/>
       <c r="D143" s="30"/>
-      <c r="E143" s="36"/>
+      <c r="E143" s="31"/>
       <c r="F143" s="36"/>
       <c r="G143" s="30"/>
       <c r="H143" s="30"/>
@@ -4063,7 +3502,7 @@
       <c r="B144" s="30"/>
       <c r="C144" s="30"/>
       <c r="D144" s="30"/>
-      <c r="E144" s="36"/>
+      <c r="E144" s="31"/>
       <c r="F144" s="36"/>
       <c r="G144" s="30"/>
       <c r="H144" s="30"/>
@@ -4074,7 +3513,7 @@
       <c r="B145" s="30"/>
       <c r="C145" s="30"/>
       <c r="D145" s="30"/>
-      <c r="E145" s="36"/>
+      <c r="E145" s="31"/>
       <c r="F145" s="36"/>
       <c r="G145" s="30"/>
       <c r="H145" s="30"/>
@@ -4085,7 +3524,7 @@
       <c r="B146" s="30"/>
       <c r="C146" s="30"/>
       <c r="D146" s="30"/>
-      <c r="E146" s="36"/>
+      <c r="E146" s="31"/>
       <c r="F146" s="36"/>
       <c r="G146" s="30"/>
       <c r="H146" s="30"/>
@@ -4096,7 +3535,7 @@
       <c r="B147" s="30"/>
       <c r="C147" s="30"/>
       <c r="D147" s="30"/>
-      <c r="E147" s="36"/>
+      <c r="E147" s="31"/>
       <c r="F147" s="36"/>
       <c r="G147" s="30"/>
       <c r="H147" s="30"/>
@@ -4107,7 +3546,7 @@
       <c r="B148" s="30"/>
       <c r="C148" s="30"/>
       <c r="D148" s="30"/>
-      <c r="E148" s="36"/>
+      <c r="E148" s="31"/>
       <c r="F148" s="36"/>
       <c r="G148" s="30"/>
       <c r="H148" s="30"/>
@@ -4118,7 +3557,7 @@
       <c r="B149" s="30"/>
       <c r="C149" s="30"/>
       <c r="D149" s="30"/>
-      <c r="E149" s="36"/>
+      <c r="E149" s="31"/>
       <c r="F149" s="36"/>
       <c r="G149" s="30"/>
       <c r="H149" s="30"/>
@@ -4129,7 +3568,7 @@
       <c r="B150" s="30"/>
       <c r="C150" s="30"/>
       <c r="D150" s="30"/>
-      <c r="E150" s="36"/>
+      <c r="E150" s="31"/>
       <c r="F150" s="36"/>
       <c r="G150" s="30"/>
       <c r="H150" s="30"/>
@@ -4140,7 +3579,7 @@
       <c r="B151" s="30"/>
       <c r="C151" s="30"/>
       <c r="D151" s="30"/>
-      <c r="E151" s="36"/>
+      <c r="E151" s="31"/>
       <c r="F151" s="36"/>
       <c r="G151" s="30"/>
       <c r="H151" s="30"/>
@@ -4151,7 +3590,7 @@
       <c r="B152" s="30"/>
       <c r="C152" s="30"/>
       <c r="D152" s="30"/>
-      <c r="E152" s="36"/>
+      <c r="E152" s="31"/>
       <c r="F152" s="36"/>
       <c r="G152" s="30"/>
       <c r="H152" s="30"/>
@@ -4162,7 +3601,7 @@
       <c r="B153" s="30"/>
       <c r="C153" s="30"/>
       <c r="D153" s="30"/>
-      <c r="E153" s="36"/>
+      <c r="E153" s="31"/>
       <c r="F153" s="36"/>
       <c r="G153" s="30"/>
       <c r="H153" s="30"/>
@@ -4173,7 +3612,7 @@
       <c r="B154" s="30"/>
       <c r="C154" s="30"/>
       <c r="D154" s="30"/>
-      <c r="E154" s="36"/>
+      <c r="E154" s="31"/>
       <c r="F154" s="36"/>
       <c r="G154" s="30"/>
       <c r="H154" s="30"/>
@@ -4184,7 +3623,7 @@
       <c r="B155" s="30"/>
       <c r="C155" s="30"/>
       <c r="D155" s="30"/>
-      <c r="E155" s="36"/>
+      <c r="E155" s="31"/>
       <c r="F155" s="36"/>
       <c r="G155" s="30"/>
       <c r="H155" s="30"/>
@@ -4195,7 +3634,7 @@
       <c r="B156" s="30"/>
       <c r="C156" s="30"/>
       <c r="D156" s="30"/>
-      <c r="E156" s="36"/>
+      <c r="E156" s="31"/>
       <c r="F156" s="36"/>
       <c r="G156" s="30"/>
       <c r="H156" s="30"/>
@@ -4206,7 +3645,7 @@
       <c r="B157" s="30"/>
       <c r="C157" s="30"/>
       <c r="D157" s="30"/>
-      <c r="E157" s="36"/>
+      <c r="E157" s="31"/>
       <c r="F157" s="36"/>
       <c r="G157" s="30"/>
       <c r="H157" s="30"/>
@@ -4217,7 +3656,7 @@
       <c r="B158" s="30"/>
       <c r="C158" s="30"/>
       <c r="D158" s="30"/>
-      <c r="E158" s="36"/>
+      <c r="E158" s="31"/>
       <c r="F158" s="36"/>
       <c r="G158" s="30"/>
       <c r="H158" s="30"/>
@@ -4228,7 +3667,7 @@
       <c r="B159" s="30"/>
       <c r="C159" s="30"/>
       <c r="D159" s="30"/>
-      <c r="E159" s="36"/>
+      <c r="E159" s="31"/>
       <c r="F159" s="36"/>
       <c r="G159" s="30"/>
       <c r="H159" s="30"/>
@@ -4239,7 +3678,7 @@
       <c r="B160" s="30"/>
       <c r="C160" s="30"/>
       <c r="D160" s="30"/>
-      <c r="E160" s="36"/>
+      <c r="E160" s="31"/>
       <c r="F160" s="36"/>
       <c r="G160" s="30"/>
       <c r="H160" s="30"/>
@@ -4250,7 +3689,7 @@
       <c r="B161" s="30"/>
       <c r="C161" s="30"/>
       <c r="D161" s="30"/>
-      <c r="E161" s="36"/>
+      <c r="E161" s="31"/>
       <c r="F161" s="36"/>
       <c r="G161" s="30"/>
       <c r="H161" s="30"/>
@@ -4261,7 +3700,7 @@
       <c r="B162" s="30"/>
       <c r="C162" s="30"/>
       <c r="D162" s="30"/>
-      <c r="E162" s="36"/>
+      <c r="E162" s="31"/>
       <c r="F162" s="36"/>
       <c r="G162" s="30"/>
       <c r="H162" s="30"/>
@@ -4272,7 +3711,7 @@
       <c r="B163" s="30"/>
       <c r="C163" s="30"/>
       <c r="D163" s="30"/>
-      <c r="E163" s="36"/>
+      <c r="E163" s="31"/>
       <c r="F163" s="36"/>
       <c r="G163" s="30"/>
       <c r="H163" s="30"/>
@@ -4283,7 +3722,7 @@
       <c r="B164" s="30"/>
       <c r="C164" s="30"/>
       <c r="D164" s="30"/>
-      <c r="E164" s="36"/>
+      <c r="E164" s="31"/>
       <c r="F164" s="36"/>
       <c r="G164" s="30"/>
       <c r="H164" s="30"/>
@@ -4294,7 +3733,7 @@
       <c r="B165" s="30"/>
       <c r="C165" s="30"/>
       <c r="D165" s="30"/>
-      <c r="E165" s="36"/>
+      <c r="E165" s="31"/>
       <c r="F165" s="36"/>
       <c r="G165" s="30"/>
       <c r="H165" s="30"/>
@@ -4305,7 +3744,7 @@
       <c r="B166" s="30"/>
       <c r="C166" s="30"/>
       <c r="D166" s="30"/>
-      <c r="E166" s="36"/>
+      <c r="E166" s="31"/>
       <c r="F166" s="36"/>
       <c r="G166" s="30"/>
       <c r="H166" s="30"/>
@@ -4316,7 +3755,7 @@
       <c r="B167" s="30"/>
       <c r="C167" s="30"/>
       <c r="D167" s="30"/>
-      <c r="E167" s="36"/>
+      <c r="E167" s="31"/>
       <c r="F167" s="36"/>
       <c r="G167" s="30"/>
       <c r="H167" s="30"/>
@@ -4327,7 +3766,7 @@
       <c r="B168" s="30"/>
       <c r="C168" s="30"/>
       <c r="D168" s="30"/>
-      <c r="E168" s="36"/>
+      <c r="E168" s="31"/>
       <c r="F168" s="36"/>
       <c r="G168" s="30"/>
       <c r="H168" s="30"/>
@@ -4338,7 +3777,7 @@
       <c r="B169" s="30"/>
       <c r="C169" s="30"/>
       <c r="D169" s="30"/>
-      <c r="E169" s="36"/>
+      <c r="E169" s="31"/>
       <c r="F169" s="36"/>
       <c r="G169" s="30"/>
       <c r="H169" s="30"/>
@@ -4349,7 +3788,7 @@
       <c r="B170" s="30"/>
       <c r="C170" s="30"/>
       <c r="D170" s="30"/>
-      <c r="E170" s="36"/>
+      <c r="E170" s="31"/>
       <c r="F170" s="36"/>
       <c r="G170" s="30"/>
       <c r="H170" s="30"/>
@@ -4360,7 +3799,7 @@
       <c r="B171" s="30"/>
       <c r="C171" s="30"/>
       <c r="D171" s="30"/>
-      <c r="E171" s="36"/>
+      <c r="E171" s="31"/>
       <c r="F171" s="36"/>
       <c r="G171" s="30"/>
       <c r="H171" s="30"/>
@@ -4371,7 +3810,7 @@
       <c r="B172" s="30"/>
       <c r="C172" s="30"/>
       <c r="D172" s="30"/>
-      <c r="E172" s="36"/>
+      <c r="E172" s="31"/>
       <c r="F172" s="36"/>
       <c r="G172" s="30"/>
       <c r="H172" s="30"/>
@@ -4382,7 +3821,7 @@
       <c r="B173" s="30"/>
       <c r="C173" s="30"/>
       <c r="D173" s="30"/>
-      <c r="E173" s="36"/>
+      <c r="E173" s="31"/>
       <c r="F173" s="36"/>
       <c r="G173" s="30"/>
       <c r="H173" s="30"/>
@@ -4393,7 +3832,7 @@
       <c r="B174" s="30"/>
       <c r="C174" s="30"/>
       <c r="D174" s="30"/>
-      <c r="E174" s="36"/>
+      <c r="E174" s="31"/>
       <c r="F174" s="36"/>
       <c r="G174" s="30"/>
       <c r="H174" s="30"/>
@@ -4404,7 +3843,7 @@
       <c r="B175" s="30"/>
       <c r="C175" s="30"/>
       <c r="D175" s="30"/>
-      <c r="E175" s="36"/>
+      <c r="E175" s="31"/>
       <c r="F175" s="36"/>
       <c r="G175" s="30"/>
       <c r="H175" s="30"/>
@@ -4415,7 +3854,7 @@
       <c r="B176" s="30"/>
       <c r="C176" s="30"/>
       <c r="D176" s="30"/>
-      <c r="E176" s="36"/>
+      <c r="E176" s="31"/>
       <c r="F176" s="36"/>
       <c r="G176" s="30"/>
       <c r="H176" s="30"/>
@@ -4426,7 +3865,7 @@
       <c r="B177" s="30"/>
       <c r="C177" s="30"/>
       <c r="D177" s="30"/>
-      <c r="E177" s="36"/>
+      <c r="E177" s="31"/>
       <c r="F177" s="36"/>
       <c r="G177" s="30"/>
       <c r="H177" s="30"/>
@@ -4437,7 +3876,7 @@
       <c r="B178" s="30"/>
       <c r="C178" s="30"/>
       <c r="D178" s="30"/>
-      <c r="E178" s="36"/>
+      <c r="E178" s="31"/>
       <c r="F178" s="36"/>
       <c r="G178" s="30"/>
       <c r="H178" s="30"/>
@@ -4448,7 +3887,7 @@
       <c r="B179" s="30"/>
       <c r="C179" s="30"/>
       <c r="D179" s="30"/>
-      <c r="E179" s="36"/>
+      <c r="E179" s="31"/>
       <c r="F179" s="36"/>
       <c r="G179" s="30"/>
       <c r="H179" s="30"/>
@@ -4459,7 +3898,7 @@
       <c r="B180" s="30"/>
       <c r="C180" s="30"/>
       <c r="D180" s="30"/>
-      <c r="E180" s="36"/>
+      <c r="E180" s="31"/>
       <c r="F180" s="36"/>
       <c r="G180" s="30"/>
       <c r="H180" s="30"/>
@@ -4470,7 +3909,7 @@
       <c r="B181" s="30"/>
       <c r="C181" s="30"/>
       <c r="D181" s="30"/>
-      <c r="E181" s="36"/>
+      <c r="E181" s="31"/>
       <c r="F181" s="36"/>
       <c r="G181" s="30"/>
       <c r="H181" s="30"/>
@@ -4481,7 +3920,7 @@
       <c r="B182" s="30"/>
       <c r="C182" s="30"/>
       <c r="D182" s="30"/>
-      <c r="E182" s="36"/>
+      <c r="E182" s="31"/>
       <c r="F182" s="36"/>
       <c r="G182" s="30"/>
       <c r="H182" s="30"/>
@@ -4492,7 +3931,7 @@
       <c r="B183" s="30"/>
       <c r="C183" s="30"/>
       <c r="D183" s="30"/>
-      <c r="E183" s="36"/>
+      <c r="E183" s="31"/>
       <c r="F183" s="36"/>
       <c r="G183" s="30"/>
       <c r="H183" s="30"/>
@@ -4503,7 +3942,7 @@
       <c r="B184" s="30"/>
       <c r="C184" s="30"/>
       <c r="D184" s="30"/>
-      <c r="E184" s="36"/>
+      <c r="E184" s="31"/>
       <c r="F184" s="36"/>
       <c r="G184" s="30"/>
       <c r="H184" s="30"/>
@@ -4514,7 +3953,7 @@
       <c r="B185" s="30"/>
       <c r="C185" s="30"/>
       <c r="D185" s="30"/>
-      <c r="E185" s="36"/>
+      <c r="E185" s="31"/>
       <c r="F185" s="36"/>
       <c r="G185" s="30"/>
       <c r="H185" s="30"/>
@@ -4525,7 +3964,7 @@
       <c r="B186" s="30"/>
       <c r="C186" s="30"/>
       <c r="D186" s="30"/>
-      <c r="E186" s="36"/>
+      <c r="E186" s="31"/>
       <c r="F186" s="36"/>
       <c r="G186" s="30"/>
       <c r="H186" s="30"/>
@@ -4536,7 +3975,7 @@
       <c r="B187" s="30"/>
       <c r="C187" s="30"/>
       <c r="D187" s="30"/>
-      <c r="E187" s="36"/>
+      <c r="E187" s="31"/>
       <c r="F187" s="36"/>
       <c r="G187" s="30"/>
       <c r="H187" s="30"/>
@@ -4547,7 +3986,7 @@
       <c r="B188" s="30"/>
       <c r="C188" s="30"/>
       <c r="D188" s="30"/>
-      <c r="E188" s="36"/>
+      <c r="E188" s="31"/>
       <c r="F188" s="36"/>
       <c r="G188" s="30"/>
       <c r="H188" s="30"/>
@@ -4558,7 +3997,7 @@
       <c r="B189" s="30"/>
       <c r="C189" s="30"/>
       <c r="D189" s="30"/>
-      <c r="E189" s="36"/>
+      <c r="E189" s="31"/>
       <c r="F189" s="36"/>
       <c r="G189" s="30"/>
       <c r="H189" s="30"/>
@@ -4569,7 +4008,7 @@
       <c r="B190" s="30"/>
       <c r="C190" s="30"/>
       <c r="D190" s="30"/>
-      <c r="E190" s="36"/>
+      <c r="E190" s="31"/>
       <c r="F190" s="36"/>
       <c r="G190" s="30"/>
       <c r="H190" s="30"/>
@@ -4580,7 +4019,7 @@
       <c r="B191" s="30"/>
       <c r="C191" s="30"/>
       <c r="D191" s="30"/>
-      <c r="E191" s="36"/>
+      <c r="E191" s="31"/>
       <c r="F191" s="36"/>
       <c r="G191" s="30"/>
       <c r="H191" s="30"/>
@@ -4591,7 +4030,7 @@
       <c r="B192" s="30"/>
       <c r="C192" s="30"/>
       <c r="D192" s="30"/>
-      <c r="E192" s="36"/>
+      <c r="E192" s="31"/>
       <c r="F192" s="36"/>
       <c r="G192" s="30"/>
       <c r="H192" s="30"/>
@@ -4602,7 +4041,7 @@
       <c r="B193" s="30"/>
       <c r="C193" s="30"/>
       <c r="D193" s="30"/>
-      <c r="E193" s="36"/>
+      <c r="E193" s="31"/>
       <c r="F193" s="36"/>
       <c r="G193" s="30"/>
       <c r="H193" s="30"/>
@@ -4613,7 +4052,7 @@
       <c r="B194" s="30"/>
       <c r="C194" s="30"/>
       <c r="D194" s="30"/>
-      <c r="E194" s="36"/>
+      <c r="E194" s="31"/>
       <c r="F194" s="36"/>
       <c r="G194" s="30"/>
       <c r="H194" s="30"/>
@@ -4624,7 +4063,7 @@
       <c r="B195" s="30"/>
       <c r="C195" s="30"/>
       <c r="D195" s="30"/>
-      <c r="E195" s="36"/>
+      <c r="E195" s="31"/>
       <c r="F195" s="36"/>
       <c r="G195" s="30"/>
       <c r="H195" s="30"/>
@@ -4635,7 +4074,7 @@
       <c r="B196" s="30"/>
       <c r="C196" s="30"/>
       <c r="D196" s="30"/>
-      <c r="E196" s="36"/>
+      <c r="E196" s="31"/>
       <c r="F196" s="36"/>
       <c r="G196" s="30"/>
       <c r="H196" s="30"/>
@@ -4646,7 +4085,7 @@
       <c r="B197" s="30"/>
       <c r="C197" s="30"/>
       <c r="D197" s="30"/>
-      <c r="E197" s="36"/>
+      <c r="E197" s="31"/>
       <c r="F197" s="36"/>
       <c r="G197" s="30"/>
       <c r="H197" s="30"/>
@@ -4657,7 +4096,7 @@
       <c r="B198" s="30"/>
       <c r="C198" s="30"/>
       <c r="D198" s="30"/>
-      <c r="E198" s="36"/>
+      <c r="E198" s="31"/>
       <c r="F198" s="36"/>
       <c r="G198" s="30"/>
       <c r="H198" s="30"/>
@@ -4668,7 +4107,7 @@
       <c r="B199" s="30"/>
       <c r="C199" s="30"/>
       <c r="D199" s="30"/>
-      <c r="E199" s="36"/>
+      <c r="E199" s="31"/>
       <c r="F199" s="36"/>
       <c r="G199" s="30"/>
       <c r="H199" s="30"/>
@@ -4679,7 +4118,7 @@
       <c r="B200" s="30"/>
       <c r="C200" s="30"/>
       <c r="D200" s="30"/>
-      <c r="E200" s="36"/>
+      <c r="E200" s="31"/>
       <c r="F200" s="36"/>
       <c r="G200" s="30"/>
       <c r="H200" s="30"/>
@@ -4690,7 +4129,7 @@
       <c r="B201" s="30"/>
       <c r="C201" s="30"/>
       <c r="D201" s="30"/>
-      <c r="E201" s="36"/>
+      <c r="E201" s="31"/>
       <c r="F201" s="36"/>
       <c r="G201" s="30"/>
       <c r="H201" s="30"/>
@@ -4701,7 +4140,7 @@
       <c r="B202" s="30"/>
       <c r="C202" s="30"/>
       <c r="D202" s="30"/>
-      <c r="E202" s="36"/>
+      <c r="E202" s="31"/>
       <c r="F202" s="36"/>
       <c r="G202" s="30"/>
       <c r="H202" s="30"/>
@@ -4712,7 +4151,7 @@
       <c r="B203" s="30"/>
       <c r="C203" s="30"/>
       <c r="D203" s="30"/>
-      <c r="E203" s="36"/>
+      <c r="E203" s="31"/>
       <c r="F203" s="36"/>
       <c r="G203" s="30"/>
       <c r="H203" s="30"/>
@@ -4723,7 +4162,7 @@
       <c r="B204" s="30"/>
       <c r="C204" s="30"/>
       <c r="D204" s="30"/>
-      <c r="E204" s="36"/>
+      <c r="E204" s="31"/>
       <c r="F204" s="36"/>
       <c r="G204" s="30"/>
       <c r="H204" s="30"/>
@@ -4734,7 +4173,7 @@
       <c r="B205" s="30"/>
       <c r="C205" s="30"/>
       <c r="D205" s="30"/>
-      <c r="E205" s="36"/>
+      <c r="E205" s="31"/>
       <c r="F205" s="36"/>
       <c r="G205" s="30"/>
       <c r="H205" s="30"/>
@@ -4745,7 +4184,7 @@
       <c r="B206" s="30"/>
       <c r="C206" s="30"/>
       <c r="D206" s="30"/>
-      <c r="E206" s="36"/>
+      <c r="E206" s="31"/>
       <c r="F206" s="36"/>
       <c r="G206" s="30"/>
       <c r="H206" s="30"/>
@@ -4756,7 +4195,7 @@
       <c r="B207" s="30"/>
       <c r="C207" s="30"/>
       <c r="D207" s="30"/>
-      <c r="E207" s="36"/>
+      <c r="E207" s="31"/>
       <c r="F207" s="36"/>
       <c r="G207" s="30"/>
       <c r="H207" s="30"/>
@@ -4767,7 +4206,7 @@
       <c r="B208" s="30"/>
       <c r="C208" s="30"/>
       <c r="D208" s="30"/>
-      <c r="E208" s="36"/>
+      <c r="E208" s="31"/>
       <c r="F208" s="36"/>
       <c r="G208" s="30"/>
       <c r="H208" s="30"/>
@@ -4778,7 +4217,7 @@
       <c r="B209" s="30"/>
       <c r="C209" s="30"/>
       <c r="D209" s="30"/>
-      <c r="E209" s="36"/>
+      <c r="E209" s="31"/>
       <c r="F209" s="36"/>
       <c r="G209" s="30"/>
       <c r="H209" s="30"/>
@@ -4789,7 +4228,7 @@
       <c r="B210" s="30"/>
       <c r="C210" s="30"/>
       <c r="D210" s="30"/>
-      <c r="E210" s="36"/>
+      <c r="E210" s="31"/>
       <c r="F210" s="36"/>
       <c r="G210" s="30"/>
       <c r="H210" s="30"/>
@@ -4800,7 +4239,7 @@
       <c r="B211" s="30"/>
       <c r="C211" s="30"/>
       <c r="D211" s="30"/>
-      <c r="E211" s="36"/>
+      <c r="E211" s="31"/>
       <c r="F211" s="36"/>
       <c r="G211" s="30"/>
       <c r="H211" s="30"/>
@@ -4811,7 +4250,7 @@
       <c r="B212" s="30"/>
       <c r="C212" s="30"/>
       <c r="D212" s="30"/>
-      <c r="E212" s="36"/>
+      <c r="E212" s="31"/>
       <c r="F212" s="36"/>
       <c r="G212" s="30"/>
       <c r="H212" s="30"/>
@@ -4822,7 +4261,7 @@
       <c r="B213" s="30"/>
       <c r="C213" s="30"/>
       <c r="D213" s="30"/>
-      <c r="E213" s="36"/>
+      <c r="E213" s="31"/>
       <c r="F213" s="36"/>
       <c r="G213" s="30"/>
       <c r="H213" s="30"/>
@@ -4833,7 +4272,7 @@
       <c r="B214" s="30"/>
       <c r="C214" s="30"/>
       <c r="D214" s="30"/>
-      <c r="E214" s="36"/>
+      <c r="E214" s="31"/>
       <c r="F214" s="36"/>
       <c r="G214" s="30"/>
       <c r="H214" s="30"/>
@@ -4844,7 +4283,7 @@
       <c r="B215" s="30"/>
       <c r="C215" s="30"/>
       <c r="D215" s="30"/>
-      <c r="E215" s="36"/>
+      <c r="E215" s="31"/>
       <c r="F215" s="36"/>
       <c r="G215" s="30"/>
       <c r="H215" s="30"/>
@@ -4855,7 +4294,7 @@
       <c r="B216" s="30"/>
       <c r="C216" s="30"/>
       <c r="D216" s="30"/>
-      <c r="E216" s="36"/>
+      <c r="E216" s="31"/>
       <c r="F216" s="36"/>
       <c r="G216" s="30"/>
       <c r="H216" s="30"/>
@@ -4866,7 +4305,7 @@
       <c r="B217" s="30"/>
       <c r="C217" s="30"/>
       <c r="D217" s="30"/>
-      <c r="E217" s="36"/>
+      <c r="E217" s="31"/>
       <c r="F217" s="36"/>
       <c r="G217" s="30"/>
       <c r="H217" s="30"/>
@@ -4877,7 +4316,7 @@
       <c r="B218" s="30"/>
       <c r="C218" s="30"/>
       <c r="D218" s="30"/>
-      <c r="E218" s="36"/>
+      <c r="E218" s="31"/>
       <c r="F218" s="36"/>
       <c r="G218" s="30"/>
       <c r="H218" s="30"/>
@@ -4888,7 +4327,7 @@
       <c r="B219" s="30"/>
       <c r="C219" s="30"/>
       <c r="D219" s="30"/>
-      <c r="E219" s="36"/>
+      <c r="E219" s="31"/>
       <c r="F219" s="36"/>
       <c r="G219" s="30"/>
       <c r="H219" s="30"/>
@@ -4899,7 +4338,7 @@
       <c r="B220" s="30"/>
       <c r="C220" s="30"/>
       <c r="D220" s="30"/>
-      <c r="E220" s="36"/>
+      <c r="E220" s="31"/>
       <c r="F220" s="36"/>
       <c r="G220" s="30"/>
       <c r="H220" s="30"/>
@@ -4910,7 +4349,7 @@
       <c r="B221" s="30"/>
       <c r="C221" s="30"/>
       <c r="D221" s="30"/>
-      <c r="E221" s="36"/>
+      <c r="E221" s="31"/>
       <c r="F221" s="36"/>
       <c r="G221" s="30"/>
       <c r="H221" s="30"/>
@@ -4921,7 +4360,7 @@
       <c r="B222" s="30"/>
       <c r="C222" s="30"/>
       <c r="D222" s="30"/>
-      <c r="E222" s="36"/>
+      <c r="E222" s="31"/>
       <c r="F222" s="36"/>
       <c r="G222" s="30"/>
       <c r="H222" s="30"/>
@@ -4932,7 +4371,7 @@
       <c r="B223" s="30"/>
       <c r="C223" s="30"/>
       <c r="D223" s="30"/>
-      <c r="E223" s="36"/>
+      <c r="E223" s="31"/>
       <c r="F223" s="36"/>
       <c r="G223" s="30"/>
       <c r="H223" s="30"/>
@@ -4943,7 +4382,7 @@
       <c r="B224" s="30"/>
       <c r="C224" s="30"/>
       <c r="D224" s="30"/>
-      <c r="E224" s="36"/>
+      <c r="E224" s="31"/>
       <c r="F224" s="36"/>
       <c r="G224" s="30"/>
       <c r="H224" s="30"/>
@@ -4954,7 +4393,7 @@
       <c r="B225" s="30"/>
       <c r="C225" s="30"/>
       <c r="D225" s="30"/>
-      <c r="E225" s="36"/>
+      <c r="E225" s="31"/>
       <c r="F225" s="36"/>
       <c r="G225" s="30"/>
       <c r="H225" s="30"/>
@@ -4965,7 +4404,7 @@
       <c r="B226" s="30"/>
       <c r="C226" s="30"/>
       <c r="D226" s="30"/>
-      <c r="E226" s="36"/>
+      <c r="E226" s="31"/>
       <c r="F226" s="36"/>
       <c r="G226" s="30"/>
       <c r="H226" s="30"/>
@@ -4976,7 +4415,7 @@
       <c r="B227" s="30"/>
       <c r="C227" s="30"/>
       <c r="D227" s="30"/>
-      <c r="E227" s="36"/>
+      <c r="E227" s="31"/>
       <c r="F227" s="36"/>
       <c r="G227" s="30"/>
       <c r="H227" s="30"/>
@@ -4987,7 +4426,7 @@
       <c r="B228" s="30"/>
       <c r="C228" s="30"/>
       <c r="D228" s="30"/>
-      <c r="E228" s="36"/>
+      <c r="E228" s="31"/>
       <c r="F228" s="36"/>
       <c r="G228" s="30"/>
       <c r="H228" s="30"/>
@@ -4998,7 +4437,7 @@
       <c r="B229" s="30"/>
       <c r="C229" s="30"/>
       <c r="D229" s="30"/>
-      <c r="E229" s="36"/>
+      <c r="E229" s="31"/>
       <c r="F229" s="36"/>
       <c r="G229" s="30"/>
       <c r="H229" s="30"/>
@@ -5009,7 +4448,7 @@
       <c r="B230" s="30"/>
       <c r="C230" s="30"/>
       <c r="D230" s="30"/>
-      <c r="E230" s="36"/>
+      <c r="E230" s="31"/>
       <c r="F230" s="36"/>
       <c r="G230" s="30"/>
       <c r="H230" s="30"/>
@@ -5020,7 +4459,7 @@
       <c r="B231" s="30"/>
       <c r="C231" s="30"/>
       <c r="D231" s="30"/>
-      <c r="E231" s="36"/>
+      <c r="E231" s="31"/>
       <c r="F231" s="36"/>
       <c r="G231" s="30"/>
       <c r="H231" s="30"/>
@@ -5031,7 +4470,7 @@
       <c r="B232" s="30"/>
       <c r="C232" s="30"/>
       <c r="D232" s="30"/>
-      <c r="E232" s="36"/>
+      <c r="E232" s="31"/>
       <c r="F232" s="36"/>
       <c r="G232" s="30"/>
       <c r="H232" s="30"/>
@@ -5042,7 +4481,7 @@
       <c r="B233" s="30"/>
       <c r="C233" s="30"/>
       <c r="D233" s="30"/>
-      <c r="E233" s="36"/>
+      <c r="E233" s="31"/>
       <c r="F233" s="36"/>
       <c r="G233" s="30"/>
       <c r="H233" s="30"/>
@@ -5053,7 +4492,7 @@
       <c r="B234" s="30"/>
       <c r="C234" s="30"/>
       <c r="D234" s="30"/>
-      <c r="E234" s="36"/>
+      <c r="E234" s="31"/>
       <c r="F234" s="36"/>
       <c r="G234" s="30"/>
       <c r="H234" s="30"/>
@@ -5064,7 +4503,7 @@
       <c r="B235" s="30"/>
       <c r="C235" s="30"/>
       <c r="D235" s="30"/>
-      <c r="E235" s="36"/>
+      <c r="E235" s="31"/>
       <c r="F235" s="36"/>
       <c r="G235" s="30"/>
       <c r="H235" s="30"/>
@@ -5075,7 +4514,7 @@
       <c r="B236" s="30"/>
       <c r="C236" s="30"/>
       <c r="D236" s="30"/>
-      <c r="E236" s="36"/>
+      <c r="E236" s="31"/>
       <c r="F236" s="36"/>
       <c r="G236" s="30"/>
       <c r="H236" s="30"/>
@@ -5086,7 +4525,7 @@
       <c r="B237" s="30"/>
       <c r="C237" s="30"/>
       <c r="D237" s="30"/>
-      <c r="E237" s="36"/>
+      <c r="E237" s="31"/>
       <c r="F237" s="36"/>
       <c r="G237" s="30"/>
       <c r="H237" s="30"/>
@@ -5097,7 +4536,7 @@
       <c r="B238" s="30"/>
       <c r="C238" s="30"/>
       <c r="D238" s="30"/>
-      <c r="E238" s="36"/>
+      <c r="E238" s="31"/>
       <c r="F238" s="36"/>
       <c r="G238" s="30"/>
       <c r="H238" s="30"/>
@@ -5108,7 +4547,7 @@
       <c r="B239" s="30"/>
       <c r="C239" s="30"/>
       <c r="D239" s="30"/>
-      <c r="E239" s="36"/>
+      <c r="E239" s="31"/>
       <c r="F239" s="36"/>
       <c r="G239" s="30"/>
       <c r="H239" s="30"/>
@@ -5119,7 +4558,7 @@
       <c r="B240" s="30"/>
       <c r="C240" s="30"/>
       <c r="D240" s="30"/>
-      <c r="E240" s="36"/>
+      <c r="E240" s="31"/>
       <c r="F240" s="36"/>
       <c r="G240" s="30"/>
       <c r="H240" s="30"/>
@@ -5130,7 +4569,7 @@
       <c r="B241" s="30"/>
       <c r="C241" s="30"/>
       <c r="D241" s="30"/>
-      <c r="E241" s="36"/>
+      <c r="E241" s="31"/>
       <c r="F241" s="36"/>
       <c r="G241" s="30"/>
       <c r="H241" s="30"/>
@@ -5141,7 +4580,7 @@
       <c r="B242" s="30"/>
       <c r="C242" s="30"/>
       <c r="D242" s="30"/>
-      <c r="E242" s="36"/>
+      <c r="E242" s="31"/>
       <c r="F242" s="36"/>
       <c r="G242" s="30"/>
       <c r="H242" s="30"/>
@@ -5152,7 +4591,7 @@
       <c r="B243" s="30"/>
       <c r="C243" s="30"/>
       <c r="D243" s="30"/>
-      <c r="E243" s="36"/>
+      <c r="E243" s="31"/>
       <c r="F243" s="36"/>
       <c r="G243" s="30"/>
       <c r="H243" s="30"/>
@@ -5163,7 +4602,7 @@
       <c r="B244" s="30"/>
       <c r="C244" s="30"/>
       <c r="D244" s="30"/>
-      <c r="E244" s="36"/>
+      <c r="E244" s="31"/>
       <c r="F244" s="36"/>
       <c r="G244" s="30"/>
       <c r="H244" s="30"/>
@@ -5174,7 +4613,7 @@
       <c r="B245" s="30"/>
       <c r="C245" s="30"/>
       <c r="D245" s="30"/>
-      <c r="E245" s="36"/>
+      <c r="E245" s="31"/>
       <c r="F245" s="36"/>
       <c r="G245" s="30"/>
       <c r="H245" s="30"/>
@@ -5185,7 +4624,7 @@
       <c r="B246" s="30"/>
       <c r="C246" s="30"/>
       <c r="D246" s="30"/>
-      <c r="E246" s="36"/>
+      <c r="E246" s="31"/>
       <c r="F246" s="36"/>
       <c r="G246" s="30"/>
       <c r="H246" s="30"/>
@@ -5196,7 +4635,7 @@
       <c r="B247" s="30"/>
       <c r="C247" s="30"/>
       <c r="D247" s="30"/>
-      <c r="E247" s="36"/>
+      <c r="E247" s="31"/>
       <c r="F247" s="36"/>
       <c r="G247" s="30"/>
       <c r="H247" s="30"/>
@@ -5207,7 +4646,7 @@
       <c r="B248" s="30"/>
       <c r="C248" s="30"/>
       <c r="D248" s="30"/>
-      <c r="E248" s="36"/>
+      <c r="E248" s="31"/>
       <c r="F248" s="36"/>
       <c r="G248" s="30"/>
       <c r="H248" s="30"/>
@@ -5218,7 +4657,7 @@
       <c r="B249" s="30"/>
       <c r="C249" s="30"/>
       <c r="D249" s="30"/>
-      <c r="E249" s="36"/>
+      <c r="E249" s="31"/>
       <c r="F249" s="36"/>
       <c r="G249" s="30"/>
       <c r="H249" s="30"/>
@@ -5229,7 +4668,7 @@
       <c r="B250" s="30"/>
       <c r="C250" s="30"/>
       <c r="D250" s="30"/>
-      <c r="E250" s="36"/>
+      <c r="E250" s="31"/>
       <c r="F250" s="36"/>
       <c r="G250" s="30"/>
       <c r="H250" s="30"/>
@@ -5240,7 +4679,7 @@
       <c r="B251" s="30"/>
       <c r="C251" s="30"/>
       <c r="D251" s="30"/>
-      <c r="E251" s="36"/>
+      <c r="E251" s="31"/>
       <c r="F251" s="36"/>
       <c r="G251" s="30"/>
       <c r="H251" s="30"/>
@@ -5251,7 +4690,7 @@
       <c r="B252" s="30"/>
       <c r="C252" s="30"/>
       <c r="D252" s="30"/>
-      <c r="E252" s="36"/>
+      <c r="E252" s="31"/>
       <c r="F252" s="36"/>
       <c r="G252" s="30"/>
       <c r="H252" s="30"/>
@@ -5262,7 +4701,7 @@
       <c r="B253" s="30"/>
       <c r="C253" s="30"/>
       <c r="D253" s="30"/>
-      <c r="E253" s="36"/>
+      <c r="E253" s="31"/>
       <c r="F253" s="36"/>
       <c r="G253" s="30"/>
       <c r="H253" s="30"/>
@@ -5273,7 +4712,7 @@
       <c r="B254" s="30"/>
       <c r="C254" s="30"/>
       <c r="D254" s="30"/>
-      <c r="E254" s="36"/>
+      <c r="E254" s="31"/>
       <c r="F254" s="36"/>
       <c r="G254" s="30"/>
       <c r="H254" s="30"/>
@@ -5284,7 +4723,7 @@
       <c r="B255" s="30"/>
       <c r="C255" s="30"/>
       <c r="D255" s="30"/>
-      <c r="E255" s="36"/>
+      <c r="E255" s="31"/>
       <c r="F255" s="36"/>
       <c r="G255" s="30"/>
       <c r="H255" s="30"/>
@@ -5295,7 +4734,7 @@
       <c r="B256" s="30"/>
       <c r="C256" s="30"/>
       <c r="D256" s="30"/>
-      <c r="E256" s="36"/>
+      <c r="E256" s="31"/>
       <c r="F256" s="36"/>
       <c r="G256" s="30"/>
       <c r="H256" s="30"/>
@@ -5306,7 +4745,7 @@
       <c r="B257" s="30"/>
       <c r="C257" s="30"/>
       <c r="D257" s="30"/>
-      <c r="E257" s="36"/>
+      <c r="E257" s="31"/>
       <c r="F257" s="36"/>
       <c r="G257" s="30"/>
       <c r="H257" s="30"/>
@@ -5317,7 +4756,7 @@
       <c r="B258" s="30"/>
       <c r="C258" s="30"/>
       <c r="D258" s="30"/>
-      <c r="E258" s="36"/>
+      <c r="E258" s="31"/>
       <c r="F258" s="36"/>
       <c r="G258" s="30"/>
       <c r="H258" s="30"/>
@@ -5328,7 +4767,7 @@
       <c r="B259" s="30"/>
       <c r="C259" s="30"/>
       <c r="D259" s="30"/>
-      <c r="E259" s="36"/>
+      <c r="E259" s="31"/>
       <c r="F259" s="36"/>
       <c r="G259" s="30"/>
       <c r="H259" s="30"/>
@@ -5339,7 +4778,7 @@
       <c r="B260" s="30"/>
       <c r="C260" s="30"/>
       <c r="D260" s="30"/>
-      <c r="E260" s="36"/>
+      <c r="E260" s="31"/>
       <c r="F260" s="36"/>
       <c r="G260" s="30"/>
       <c r="H260" s="30"/>
@@ -5350,7 +4789,7 @@
       <c r="B261" s="30"/>
       <c r="C261" s="30"/>
       <c r="D261" s="30"/>
-      <c r="E261" s="36"/>
+      <c r="E261" s="31"/>
       <c r="F261" s="36"/>
       <c r="G261" s="30"/>
       <c r="H261" s="30"/>
@@ -5361,7 +4800,7 @@
       <c r="B262" s="30"/>
       <c r="C262" s="30"/>
       <c r="D262" s="30"/>
-      <c r="E262" s="36"/>
+      <c r="E262" s="31"/>
       <c r="F262" s="36"/>
       <c r="G262" s="30"/>
       <c r="H262" s="30"/>
@@ -5372,7 +4811,7 @@
       <c r="B263" s="30"/>
       <c r="C263" s="30"/>
       <c r="D263" s="30"/>
-      <c r="E263" s="36"/>
+      <c r="E263" s="31"/>
       <c r="F263" s="36"/>
       <c r="G263" s="30"/>
       <c r="H263" s="30"/>
@@ -5383,7 +4822,7 @@
       <c r="B264" s="30"/>
       <c r="C264" s="30"/>
       <c r="D264" s="30"/>
-      <c r="E264" s="36"/>
+      <c r="E264" s="31"/>
       <c r="F264" s="36"/>
       <c r="G264" s="30"/>
       <c r="H264" s="30"/>
@@ -5394,7 +4833,7 @@
       <c r="B265" s="30"/>
       <c r="C265" s="30"/>
       <c r="D265" s="30"/>
-      <c r="E265" s="36"/>
+      <c r="E265" s="31"/>
       <c r="F265" s="36"/>
       <c r="G265" s="30"/>
       <c r="H265" s="30"/>
@@ -5405,7 +4844,7 @@
       <c r="B266" s="30"/>
       <c r="C266" s="30"/>
       <c r="D266" s="30"/>
-      <c r="E266" s="36"/>
+      <c r="E266" s="31"/>
       <c r="F266" s="36"/>
       <c r="G266" s="30"/>
       <c r="H266" s="30"/>
@@ -5416,7 +4855,7 @@
       <c r="B267" s="30"/>
       <c r="C267" s="30"/>
       <c r="D267" s="30"/>
-      <c r="E267" s="36"/>
+      <c r="E267" s="31"/>
       <c r="F267" s="36"/>
       <c r="G267" s="30"/>
       <c r="H267" s="30"/>
@@ -5427,7 +4866,7 @@
       <c r="B268" s="30"/>
       <c r="C268" s="30"/>
       <c r="D268" s="30"/>
-      <c r="E268" s="36"/>
+      <c r="E268" s="31"/>
       <c r="F268" s="36"/>
       <c r="G268" s="30"/>
       <c r="H268" s="30"/>
@@ -5438,7 +4877,7 @@
       <c r="B269" s="30"/>
       <c r="C269" s="30"/>
       <c r="D269" s="30"/>
-      <c r="E269" s="36"/>
+      <c r="E269" s="31"/>
       <c r="F269" s="36"/>
       <c r="G269" s="30"/>
       <c r="H269" s="30"/>
@@ -5449,7 +4888,7 @@
       <c r="B270" s="30"/>
       <c r="C270" s="30"/>
       <c r="D270" s="30"/>
-      <c r="E270" s="36"/>
+      <c r="E270" s="31"/>
       <c r="F270" s="36"/>
       <c r="G270" s="30"/>
       <c r="H270" s="30"/>
@@ -5460,7 +4899,7 @@
       <c r="B271" s="30"/>
       <c r="C271" s="30"/>
       <c r="D271" s="30"/>
-      <c r="E271" s="36"/>
+      <c r="E271" s="31"/>
       <c r="F271" s="36"/>
       <c r="G271" s="30"/>
       <c r="H271" s="30"/>
@@ -5471,7 +4910,7 @@
       <c r="B272" s="30"/>
       <c r="C272" s="30"/>
       <c r="D272" s="30"/>
-      <c r="E272" s="36"/>
+      <c r="E272" s="31"/>
       <c r="F272" s="36"/>
       <c r="G272" s="30"/>
       <c r="H272" s="30"/>
@@ -5482,7 +4921,7 @@
       <c r="B273" s="30"/>
       <c r="C273" s="30"/>
       <c r="D273" s="30"/>
-      <c r="E273" s="36"/>
+      <c r="E273" s="31"/>
       <c r="F273" s="36"/>
       <c r="G273" s="30"/>
       <c r="H273" s="30"/>
@@ -5493,7 +4932,7 @@
       <c r="B274" s="30"/>
       <c r="C274" s="30"/>
       <c r="D274" s="30"/>
-      <c r="E274" s="36"/>
+      <c r="E274" s="31"/>
       <c r="F274" s="36"/>
       <c r="G274" s="30"/>
       <c r="H274" s="30"/>
@@ -5504,7 +4943,7 @@
       <c r="B275" s="30"/>
       <c r="C275" s="30"/>
       <c r="D275" s="30"/>
-      <c r="E275" s="36"/>
+      <c r="E275" s="31"/>
       <c r="F275" s="36"/>
       <c r="G275" s="30"/>
       <c r="H275" s="30"/>
@@ -5515,7 +4954,7 @@
       <c r="B276" s="30"/>
       <c r="C276" s="30"/>
       <c r="D276" s="30"/>
-      <c r="E276" s="36"/>
+      <c r="E276" s="31"/>
       <c r="F276" s="36"/>
       <c r="G276" s="30"/>
       <c r="H276" s="30"/>
@@ -5526,7 +4965,7 @@
       <c r="B277" s="30"/>
       <c r="C277" s="30"/>
       <c r="D277" s="30"/>
-      <c r="E277" s="36"/>
+      <c r="E277" s="31"/>
       <c r="F277" s="36"/>
       <c r="G277" s="30"/>
       <c r="H277" s="30"/>
@@ -5537,7 +4976,7 @@
       <c r="B278" s="30"/>
       <c r="C278" s="30"/>
       <c r="D278" s="30"/>
-      <c r="E278" s="36"/>
+      <c r="E278" s="31"/>
       <c r="F278" s="36"/>
       <c r="G278" s="30"/>
       <c r="H278" s="30"/>
@@ -5548,7 +4987,7 @@
       <c r="B279" s="30"/>
       <c r="C279" s="30"/>
       <c r="D279" s="30"/>
-      <c r="E279" s="36"/>
+      <c r="E279" s="31"/>
       <c r="F279" s="36"/>
       <c r="G279" s="30"/>
       <c r="H279" s="30"/>
@@ -5559,7 +4998,7 @@
       <c r="B280" s="30"/>
       <c r="C280" s="30"/>
       <c r="D280" s="30"/>
-      <c r="E280" s="36"/>
+      <c r="E280" s="31"/>
       <c r="F280" s="36"/>
       <c r="G280" s="30"/>
       <c r="H280" s="30"/>
@@ -5570,7 +5009,7 @@
       <c r="B281" s="30"/>
       <c r="C281" s="30"/>
       <c r="D281" s="30"/>
-      <c r="E281" s="36"/>
+      <c r="E281" s="31"/>
       <c r="F281" s="36"/>
       <c r="G281" s="30"/>
       <c r="H281" s="30"/>
@@ -5581,7 +5020,7 @@
       <c r="B282" s="30"/>
       <c r="C282" s="30"/>
       <c r="D282" s="30"/>
-      <c r="E282" s="36"/>
+      <c r="E282" s="31"/>
       <c r="F282" s="36"/>
       <c r="G282" s="30"/>
       <c r="H282" s="30"/>
@@ -5592,7 +5031,7 @@
       <c r="B283" s="30"/>
       <c r="C283" s="30"/>
       <c r="D283" s="30"/>
-      <c r="E283" s="36"/>
+      <c r="E283" s="31"/>
       <c r="F283" s="36"/>
       <c r="G283" s="30"/>
       <c r="H283" s="30"/>
@@ -5603,7 +5042,7 @@
       <c r="B284" s="30"/>
       <c r="C284" s="30"/>
       <c r="D284" s="30"/>
-      <c r="E284" s="36"/>
+      <c r="E284" s="31"/>
       <c r="F284" s="36"/>
       <c r="G284" s="30"/>
       <c r="H284" s="30"/>
@@ -5614,7 +5053,7 @@
       <c r="B285" s="30"/>
       <c r="C285" s="30"/>
       <c r="D285" s="30"/>
-      <c r="E285" s="36"/>
+      <c r="E285" s="31"/>
       <c r="F285" s="36"/>
       <c r="G285" s="30"/>
       <c r="H285" s="30"/>
@@ -5625,7 +5064,7 @@
       <c r="B286" s="30"/>
       <c r="C286" s="30"/>
       <c r="D286" s="30"/>
-      <c r="E286" s="36"/>
+      <c r="E286" s="31"/>
       <c r="F286" s="36"/>
       <c r="G286" s="30"/>
       <c r="H286" s="30"/>
@@ -5636,7 +5075,7 @@
       <c r="B287" s="30"/>
       <c r="C287" s="30"/>
       <c r="D287" s="30"/>
-      <c r="E287" s="36"/>
+      <c r="E287" s="31"/>
       <c r="F287" s="36"/>
       <c r="G287" s="30"/>
       <c r="H287" s="30"/>
@@ -5647,7 +5086,7 @@
       <c r="B288" s="30"/>
       <c r="C288" s="30"/>
       <c r="D288" s="30"/>
-      <c r="E288" s="36"/>
+      <c r="E288" s="31"/>
       <c r="F288" s="36"/>
       <c r="G288" s="30"/>
       <c r="H288" s="30"/>
@@ -5658,7 +5097,7 @@
       <c r="B289" s="30"/>
       <c r="C289" s="30"/>
       <c r="D289" s="30"/>
-      <c r="E289" s="36"/>
+      <c r="E289" s="31"/>
       <c r="F289" s="36"/>
       <c r="G289" s="30"/>
       <c r="H289" s="30"/>
@@ -5669,7 +5108,7 @@
       <c r="B290" s="30"/>
       <c r="C290" s="30"/>
       <c r="D290" s="30"/>
-      <c r="E290" s="36"/>
+      <c r="E290" s="31"/>
       <c r="F290" s="36"/>
       <c r="G290" s="30"/>
       <c r="H290" s="30"/>
@@ -5680,7 +5119,7 @@
       <c r="B291" s="30"/>
       <c r="C291" s="30"/>
       <c r="D291" s="30"/>
-      <c r="E291" s="36"/>
+      <c r="E291" s="31"/>
       <c r="F291" s="36"/>
       <c r="G291" s="30"/>
       <c r="H291" s="30"/>
@@ -5691,7 +5130,7 @@
       <c r="B292" s="30"/>
       <c r="C292" s="30"/>
       <c r="D292" s="30"/>
-      <c r="E292" s="36"/>
+      <c r="E292" s="31"/>
       <c r="F292" s="36"/>
       <c r="G292" s="30"/>
       <c r="H292" s="30"/>
@@ -5702,7 +5141,7 @@
       <c r="B293" s="30"/>
       <c r="C293" s="30"/>
       <c r="D293" s="30"/>
-      <c r="E293" s="36"/>
+      <c r="E293" s="31"/>
       <c r="F293" s="36"/>
       <c r="G293" s="30"/>
       <c r="H293" s="30"/>
@@ -5713,7 +5152,7 @@
       <c r="B294" s="30"/>
       <c r="C294" s="30"/>
       <c r="D294" s="30"/>
-      <c r="E294" s="36"/>
+      <c r="E294" s="31"/>
       <c r="F294" s="36"/>
       <c r="G294" s="30"/>
       <c r="H294" s="30"/>
@@ -5724,7 +5163,7 @@
       <c r="B295" s="30"/>
       <c r="C295" s="30"/>
       <c r="D295" s="30"/>
-      <c r="E295" s="36"/>
+      <c r="E295" s="31"/>
       <c r="F295" s="36"/>
       <c r="G295" s="30"/>
       <c r="H295" s="30"/>
@@ -5735,7 +5174,7 @@
       <c r="B296" s="30"/>
       <c r="C296" s="30"/>
       <c r="D296" s="30"/>
-      <c r="E296" s="36"/>
+      <c r="E296" s="31"/>
       <c r="F296" s="36"/>
       <c r="G296" s="30"/>
       <c r="H296" s="30"/>
@@ -5746,7 +5185,7 @@
       <c r="B297" s="30"/>
       <c r="C297" s="30"/>
       <c r="D297" s="30"/>
-      <c r="E297" s="36"/>
+      <c r="E297" s="31"/>
       <c r="F297" s="36"/>
       <c r="G297" s="30"/>
       <c r="H297" s="30"/>
@@ -5757,7 +5196,7 @@
       <c r="B298" s="30"/>
       <c r="C298" s="30"/>
       <c r="D298" s="30"/>
-      <c r="E298" s="36"/>
+      <c r="E298" s="31"/>
       <c r="F298" s="36"/>
       <c r="G298" s="30"/>
       <c r="H298" s="30"/>
@@ -5768,7 +5207,7 @@
       <c r="B299" s="30"/>
       <c r="C299" s="30"/>
       <c r="D299" s="30"/>
-      <c r="E299" s="36"/>
+      <c r="E299" s="31"/>
       <c r="F299" s="36"/>
       <c r="G299" s="30"/>
       <c r="H299" s="30"/>
@@ -5779,7 +5218,7 @@
       <c r="B300" s="30"/>
       <c r="C300" s="30"/>
       <c r="D300" s="30"/>
-      <c r="E300" s="36"/>
+      <c r="E300" s="31"/>
       <c r="F300" s="36"/>
       <c r="G300" s="30"/>
       <c r="H300" s="30"/>
@@ -5790,7 +5229,7 @@
       <c r="B301" s="30"/>
       <c r="C301" s="30"/>
       <c r="D301" s="30"/>
-      <c r="E301" s="36"/>
+      <c r="E301" s="31"/>
       <c r="F301" s="36"/>
       <c r="G301" s="30"/>
       <c r="H301" s="30"/>
@@ -5801,7 +5240,7 @@
       <c r="B302" s="30"/>
       <c r="C302" s="30"/>
       <c r="D302" s="30"/>
-      <c r="E302" s="36"/>
+      <c r="E302" s="31"/>
       <c r="F302" s="36"/>
       <c r="G302" s="30"/>
       <c r="H302" s="30"/>
@@ -5812,7 +5251,7 @@
       <c r="B303" s="30"/>
       <c r="C303" s="30"/>
       <c r="D303" s="30"/>
-      <c r="E303" s="36"/>
+      <c r="E303" s="31"/>
       <c r="F303" s="36"/>
       <c r="G303" s="30"/>
       <c r="H303" s="30"/>
@@ -5823,7 +5262,7 @@
       <c r="B304" s="30"/>
       <c r="C304" s="30"/>
       <c r="D304" s="30"/>
-      <c r="E304" s="36"/>
+      <c r="E304" s="31"/>
       <c r="F304" s="36"/>
       <c r="G304" s="30"/>
       <c r="H304" s="30"/>
@@ -5834,7 +5273,7 @@
       <c r="B305" s="30"/>
       <c r="C305" s="30"/>
       <c r="D305" s="30"/>
-      <c r="E305" s="36"/>
+      <c r="E305" s="31"/>
       <c r="F305" s="36"/>
       <c r="G305" s="30"/>
       <c r="H305" s="30"/>
@@ -5845,7 +5284,7 @@
       <c r="B306" s="30"/>
       <c r="C306" s="30"/>
       <c r="D306" s="30"/>
-      <c r="E306" s="36"/>
+      <c r="E306" s="31"/>
       <c r="F306" s="36"/>
       <c r="G306" s="30"/>
       <c r="H306" s="30"/>
@@ -5856,7 +5295,7 @@
       <c r="B307" s="30"/>
       <c r="C307" s="30"/>
       <c r="D307" s="30"/>
-      <c r="E307" s="36"/>
+      <c r="E307" s="31"/>
       <c r="F307" s="36"/>
       <c r="G307" s="30"/>
       <c r="H307" s="30"/>
@@ -5867,7 +5306,7 @@
       <c r="B308" s="30"/>
       <c r="C308" s="30"/>
       <c r="D308" s="30"/>
-      <c r="E308" s="36"/>
+      <c r="E308" s="31"/>
       <c r="F308" s="36"/>
       <c r="G308" s="30"/>
       <c r="H308" s="30"/>
@@ -5878,7 +5317,7 @@
       <c r="B309" s="30"/>
       <c r="C309" s="30"/>
       <c r="D309" s="30"/>
-      <c r="E309" s="36"/>
+      <c r="E309" s="31"/>
       <c r="F309" s="36"/>
       <c r="G309" s="30"/>
       <c r="H309" s="30"/>
@@ -5889,7 +5328,7 @@
       <c r="B310" s="30"/>
       <c r="C310" s="30"/>
       <c r="D310" s="30"/>
-      <c r="E310" s="36"/>
+      <c r="E310" s="31"/>
       <c r="F310" s="36"/>
       <c r="G310" s="30"/>
       <c r="H310" s="30"/>
@@ -5900,7 +5339,7 @@
       <c r="B311" s="30"/>
       <c r="C311" s="30"/>
       <c r="D311" s="30"/>
-      <c r="E311" s="36"/>
+      <c r="E311" s="31"/>
       <c r="F311" s="36"/>
       <c r="G311" s="30"/>
       <c r="H311" s="30"/>
@@ -5911,7 +5350,7 @@
       <c r="B312" s="30"/>
       <c r="C312" s="30"/>
       <c r="D312" s="30"/>
-      <c r="E312" s="36"/>
+      <c r="E312" s="31"/>
       <c r="F312" s="36"/>
       <c r="G312" s="30"/>
       <c r="H312" s="30"/>
@@ -5922,7 +5361,7 @@
       <c r="B313" s="30"/>
       <c r="C313" s="30"/>
       <c r="D313" s="30"/>
-      <c r="E313" s="36"/>
+      <c r="E313" s="31"/>
       <c r="F313" s="36"/>
       <c r="G313" s="30"/>
       <c r="H313" s="30"/>
@@ -5933,7 +5372,7 @@
       <c r="B314" s="30"/>
       <c r="C314" s="30"/>
       <c r="D314" s="30"/>
-      <c r="E314" s="36"/>
+      <c r="E314" s="31"/>
       <c r="F314" s="36"/>
       <c r="G314" s="30"/>
       <c r="H314" s="30"/>
@@ -5944,7 +5383,7 @@
       <c r="B315" s="30"/>
       <c r="C315" s="30"/>
       <c r="D315" s="30"/>
-      <c r="E315" s="36"/>
+      <c r="E315" s="31"/>
       <c r="F315" s="36"/>
       <c r="G315" s="30"/>
       <c r="H315" s="30"/>
@@ -5955,7 +5394,7 @@
       <c r="B316" s="30"/>
       <c r="C316" s="30"/>
       <c r="D316" s="30"/>
-      <c r="E316" s="36"/>
+      <c r="E316" s="31"/>
       <c r="F316" s="36"/>
       <c r="G316" s="30"/>
       <c r="H316" s="30"/>
@@ -5966,7 +5405,7 @@
       <c r="B317" s="30"/>
       <c r="C317" s="30"/>
       <c r="D317" s="30"/>
-      <c r="E317" s="36"/>
+      <c r="E317" s="31"/>
       <c r="F317" s="36"/>
       <c r="G317" s="30"/>
       <c r="H317" s="30"/>
@@ -5977,7 +5416,7 @@
       <c r="B318" s="30"/>
       <c r="C318" s="30"/>
       <c r="D318" s="30"/>
-      <c r="E318" s="36"/>
+      <c r="E318" s="31"/>
       <c r="F318" s="36"/>
       <c r="G318" s="30"/>
       <c r="H318" s="30"/>
@@ -5988,7 +5427,7 @@
       <c r="B319" s="30"/>
       <c r="C319" s="30"/>
       <c r="D319" s="30"/>
-      <c r="E319" s="36"/>
+      <c r="E319" s="31"/>
       <c r="F319" s="36"/>
       <c r="G319" s="30"/>
       <c r="H319" s="30"/>
@@ -5999,7 +5438,7 @@
       <c r="B320" s="30"/>
       <c r="C320" s="30"/>
       <c r="D320" s="30"/>
-      <c r="E320" s="36"/>
+      <c r="E320" s="31"/>
       <c r="F320" s="36"/>
       <c r="G320" s="30"/>
       <c r="H320" s="30"/>
@@ -6010,7 +5449,7 @@
       <c r="B321" s="30"/>
       <c r="C321" s="30"/>
       <c r="D321" s="30"/>
-      <c r="E321" s="36"/>
+      <c r="E321" s="31"/>
       <c r="F321" s="36"/>
       <c r="G321" s="30"/>
       <c r="H321" s="30"/>
@@ -6021,7 +5460,7 @@
       <c r="B322" s="30"/>
       <c r="C322" s="30"/>
       <c r="D322" s="30"/>
-      <c r="E322" s="36"/>
+      <c r="E322" s="31"/>
       <c r="F322" s="36"/>
       <c r="G322" s="30"/>
       <c r="H322" s="30"/>
@@ -6032,7 +5471,7 @@
       <c r="B323" s="30"/>
       <c r="C323" s="30"/>
       <c r="D323" s="30"/>
-      <c r="E323" s="36"/>
+      <c r="E323" s="31"/>
       <c r="F323" s="36"/>
       <c r="G323" s="30"/>
       <c r="H323" s="30"/>
@@ -6043,7 +5482,7 @@
       <c r="B324" s="30"/>
       <c r="C324" s="30"/>
       <c r="D324" s="30"/>
-      <c r="E324" s="36"/>
+      <c r="E324" s="31"/>
       <c r="F324" s="36"/>
       <c r="G324" s="30"/>
       <c r="H324" s="30"/>
@@ -6054,7 +5493,7 @@
       <c r="B325" s="30"/>
       <c r="C325" s="30"/>
       <c r="D325" s="30"/>
-      <c r="E325" s="36"/>
+      <c r="E325" s="31"/>
       <c r="F325" s="36"/>
       <c r="G325" s="30"/>
       <c r="H325" s="30"/>
@@ -6065,7 +5504,7 @@
       <c r="B326" s="30"/>
       <c r="C326" s="30"/>
       <c r="D326" s="30"/>
-      <c r="E326" s="36"/>
+      <c r="E326" s="31"/>
       <c r="F326" s="36"/>
       <c r="G326" s="30"/>
       <c r="H326" s="30"/>
@@ -6076,7 +5515,7 @@
       <c r="B327" s="30"/>
       <c r="C327" s="30"/>
       <c r="D327" s="30"/>
-      <c r="E327" s="36"/>
+      <c r="E327" s="31"/>
       <c r="F327" s="36"/>
       <c r="G327" s="30"/>
       <c r="H327" s="30"/>
@@ -6087,7 +5526,7 @@
       <c r="B328" s="30"/>
       <c r="C328" s="30"/>
       <c r="D328" s="30"/>
-      <c r="E328" s="36"/>
+      <c r="E328" s="31"/>
       <c r="F328" s="36"/>
       <c r="G328" s="30"/>
       <c r="H328" s="30"/>
@@ -6098,7 +5537,7 @@
       <c r="B329" s="30"/>
       <c r="C329" s="30"/>
       <c r="D329" s="30"/>
-      <c r="E329" s="36"/>
+      <c r="E329" s="31"/>
       <c r="F329" s="36"/>
       <c r="G329" s="30"/>
       <c r="H329" s="30"/>
@@ -6109,7 +5548,7 @@
       <c r="B330" s="30"/>
       <c r="C330" s="30"/>
       <c r="D330" s="30"/>
-      <c r="E330" s="36"/>
+      <c r="E330" s="31"/>
       <c r="F330" s="36"/>
       <c r="G330" s="30"/>
       <c r="H330" s="30"/>
@@ -6120,7 +5559,7 @@
       <c r="B331" s="30"/>
       <c r="C331" s="30"/>
       <c r="D331" s="30"/>
-      <c r="E331" s="36"/>
+      <c r="E331" s="31"/>
       <c r="F331" s="36"/>
       <c r="G331" s="30"/>
       <c r="H331" s="30"/>
@@ -6131,7 +5570,7 @@
       <c r="B332" s="30"/>
       <c r="C332" s="30"/>
       <c r="D332" s="30"/>
-      <c r="E332" s="36"/>
+      <c r="E332" s="31"/>
       <c r="F332" s="36"/>
       <c r="G332" s="30"/>
       <c r="H332" s="30"/>
@@ -6142,7 +5581,7 @@
       <c r="B333" s="30"/>
       <c r="C333" s="30"/>
       <c r="D333" s="30"/>
-      <c r="E333" s="36"/>
+      <c r="E333" s="31"/>
       <c r="F333" s="36"/>
       <c r="G333" s="30"/>
       <c r="H333" s="30"/>
@@ -6153,7 +5592,7 @@
       <c r="B334" s="30"/>
       <c r="C334" s="30"/>
       <c r="D334" s="30"/>
-      <c r="E334" s="36"/>
+      <c r="E334" s="31"/>
       <c r="F334" s="36"/>
       <c r="G334" s="30"/>
       <c r="H334" s="30"/>
@@ -6164,7 +5603,7 @@
       <c r="B335" s="30"/>
       <c r="C335" s="30"/>
       <c r="D335" s="30"/>
-      <c r="E335" s="36"/>
+      <c r="E335" s="31"/>
       <c r="F335" s="36"/>
       <c r="G335" s="30"/>
       <c r="H335" s="30"/>
@@ -6175,7 +5614,7 @@
       <c r="B336" s="30"/>
       <c r="C336" s="30"/>
       <c r="D336" s="30"/>
-      <c r="E336" s="36"/>
+      <c r="E336" s="31"/>
       <c r="F336" s="36"/>
       <c r="G336" s="30"/>
       <c r="H336" s="30"/>
@@ -6186,7 +5625,7 @@
       <c r="B337" s="30"/>
       <c r="C337" s="30"/>
       <c r="D337" s="30"/>
-      <c r="E337" s="36"/>
+      <c r="E337" s="31"/>
       <c r="F337" s="36"/>
       <c r="G337" s="30"/>
       <c r="H337" s="30"/>
@@ -6197,7 +5636,7 @@
       <c r="B338" s="30"/>
       <c r="C338" s="30"/>
       <c r="D338" s="30"/>
-      <c r="E338" s="36"/>
+      <c r="E338" s="31"/>
       <c r="F338" s="36"/>
       <c r="G338" s="30"/>
       <c r="H338" s="30"/>
@@ -6208,7 +5647,7 @@
       <c r="B339" s="30"/>
       <c r="C339" s="30"/>
       <c r="D339" s="30"/>
-      <c r="E339" s="36"/>
+      <c r="E339" s="31"/>
       <c r="F339" s="36"/>
       <c r="G339" s="30"/>
       <c r="H339" s="30"/>
@@ -6219,7 +5658,7 @@
       <c r="B340" s="30"/>
       <c r="C340" s="30"/>
       <c r="D340" s="30"/>
-      <c r="E340" s="36"/>
+      <c r="E340" s="31"/>
       <c r="F340" s="36"/>
       <c r="G340" s="30"/>
       <c r="H340" s="30"/>
@@ -6230,7 +5669,7 @@
       <c r="B341" s="30"/>
       <c r="C341" s="30"/>
       <c r="D341" s="30"/>
-      <c r="E341" s="36"/>
+      <c r="E341" s="31"/>
       <c r="F341" s="36"/>
       <c r="G341" s="30"/>
       <c r="H341" s="30"/>
@@ -6241,7 +5680,7 @@
       <c r="B342" s="30"/>
       <c r="C342" s="30"/>
       <c r="D342" s="30"/>
-      <c r="E342" s="36"/>
+      <c r="E342" s="31"/>
       <c r="F342" s="36"/>
       <c r="G342" s="30"/>
       <c r="H342" s="30"/>
@@ -6252,7 +5691,7 @@
       <c r="B343" s="30"/>
       <c r="C343" s="30"/>
       <c r="D343" s="30"/>
-      <c r="E343" s="36"/>
+      <c r="E343" s="31"/>
       <c r="F343" s="36"/>
       <c r="G343" s="30"/>
       <c r="H343" s="30"/>
@@ -6263,7 +5702,7 @@
       <c r="B344" s="30"/>
       <c r="C344" s="30"/>
       <c r="D344" s="30"/>
-      <c r="E344" s="36"/>
+      <c r="E344" s="31"/>
       <c r="F344" s="36"/>
       <c r="G344" s="30"/>
       <c r="H344" s="30"/>
@@ -6274,7 +5713,7 @@
       <c r="B345" s="30"/>
       <c r="C345" s="30"/>
       <c r="D345" s="30"/>
-      <c r="E345" s="36"/>
+      <c r="E345" s="31"/>
       <c r="F345" s="36"/>
       <c r="G345" s="30"/>
       <c r="H345" s="30"/>
@@ -6285,7 +5724,7 @@
       <c r="B346" s="30"/>
       <c r="C346" s="30"/>
       <c r="D346" s="30"/>
-      <c r="E346" s="36"/>
+      <c r="E346" s="31"/>
       <c r="F346" s="36"/>
       <c r="G346" s="30"/>
       <c r="H346" s="30"/>
@@ -6296,7 +5735,7 @@
       <c r="B347" s="30"/>
       <c r="C347" s="30"/>
       <c r="D347" s="30"/>
-      <c r="E347" s="36"/>
+      <c r="E347" s="31"/>
       <c r="F347" s="36"/>
       <c r="G347" s="30"/>
       <c r="H347" s="30"/>
@@ -6307,7 +5746,7 @@
       <c r="B348" s="30"/>
       <c r="C348" s="30"/>
       <c r="D348" s="30"/>
-      <c r="E348" s="36"/>
+      <c r="E348" s="31"/>
       <c r="F348" s="36"/>
       <c r="G348" s="30"/>
       <c r="H348" s="30"/>
@@ -6318,7 +5757,7 @@
       <c r="B349" s="30"/>
       <c r="C349" s="30"/>
       <c r="D349" s="30"/>
-      <c r="E349" s="36"/>
+      <c r="E349" s="31"/>
       <c r="F349" s="36"/>
       <c r="G349" s="30"/>
       <c r="H349" s="30"/>
@@ -6329,7 +5768,7 @@
       <c r="B350" s="30"/>
       <c r="C350" s="30"/>
       <c r="D350" s="30"/>
-      <c r="E350" s="36"/>
+      <c r="E350" s="31"/>
       <c r="F350" s="36"/>
       <c r="G350" s="30"/>
       <c r="H350" s="30"/>
@@ -6340,7 +5779,7 @@
       <c r="B351" s="30"/>
       <c r="C351" s="30"/>
       <c r="D351" s="30"/>
-      <c r="E351" s="36"/>
+      <c r="E351" s="31"/>
       <c r="F351" s="36"/>
       <c r="G351" s="30"/>
       <c r="H351" s="30"/>
@@ -6351,7 +5790,7 @@
       <c r="B352" s="30"/>
       <c r="C352" s="30"/>
       <c r="D352" s="30"/>
-      <c r="E352" s="36"/>
+      <c r="E352" s="31"/>
       <c r="F352" s="36"/>
       <c r="G352" s="30"/>
       <c r="H352" s="30"/>
@@ -6362,7 +5801,7 @@
       <c r="B353" s="30"/>
       <c r="C353" s="30"/>
       <c r="D353" s="30"/>
-      <c r="E353" s="36"/>
+      <c r="E353" s="31"/>
       <c r="F353" s="36"/>
       <c r="G353" s="30"/>
       <c r="H353" s="30"/>
@@ -6373,7 +5812,7 @@
       <c r="B354" s="30"/>
       <c r="C354" s="30"/>
       <c r="D354" s="30"/>
-      <c r="E354" s="36"/>
+      <c r="E354" s="31"/>
       <c r="F354" s="36"/>
       <c r="G354" s="30"/>
       <c r="H354" s="30"/>
@@ -6384,7 +5823,7 @@
       <c r="B355" s="30"/>
       <c r="C355" s="30"/>
       <c r="D355" s="30"/>
-      <c r="E355" s="36"/>
+      <c r="E355" s="31"/>
       <c r="F355" s="36"/>
       <c r="G355" s="30"/>
       <c r="H355" s="30"/>
@@ -6395,7 +5834,7 @@
       <c r="B356" s="30"/>
       <c r="C356" s="30"/>
       <c r="D356" s="30"/>
-      <c r="E356" s="36"/>
+      <c r="E356" s="31"/>
       <c r="F356" s="36"/>
       <c r="G356" s="30"/>
       <c r="H356" s="30"/>
@@ -6406,7 +5845,7 @@
       <c r="B357" s="30"/>
       <c r="C357" s="30"/>
       <c r="D357" s="30"/>
-      <c r="E357" s="36"/>
+      <c r="E357" s="31"/>
       <c r="F357" s="36"/>
       <c r="G357" s="30"/>
       <c r="H357" s="30"/>
@@ -6417,7 +5856,7 @@
       <c r="B358" s="30"/>
       <c r="C358" s="30"/>
       <c r="D358" s="30"/>
-      <c r="E358" s="36"/>
+      <c r="E358" s="31"/>
       <c r="F358" s="36"/>
       <c r="G358" s="30"/>
       <c r="H358" s="30"/>
@@ -6428,7 +5867,7 @@
       <c r="B359" s="30"/>
       <c r="C359" s="30"/>
       <c r="D359" s="30"/>
-      <c r="E359" s="36"/>
+      <c r="E359" s="31"/>
       <c r="F359" s="36"/>
       <c r="G359" s="30"/>
       <c r="H359" s="30"/>
@@ -6439,7 +5878,7 @@
       <c r="B360" s="30"/>
       <c r="C360" s="30"/>
       <c r="D360" s="30"/>
-      <c r="E360" s="36"/>
+      <c r="E360" s="31"/>
       <c r="F360" s="36"/>
       <c r="G360" s="30"/>
       <c r="H360" s="30"/>
@@ -6450,7 +5889,7 @@
       <c r="B361" s="30"/>
       <c r="C361" s="30"/>
       <c r="D361" s="30"/>
-      <c r="E361" s="36"/>
+      <c r="E361" s="31"/>
       <c r="F361" s="36"/>
       <c r="G361" s="30"/>
       <c r="H361" s="30"/>
@@ -6461,7 +5900,7 @@
       <c r="B362" s="30"/>
       <c r="C362" s="30"/>
       <c r="D362" s="30"/>
-      <c r="E362" s="36"/>
+      <c r="E362" s="31"/>
       <c r="F362" s="36"/>
       <c r="G362" s="30"/>
       <c r="H362" s="30"/>
@@ -6472,7 +5911,7 @@
       <c r="B363" s="30"/>
       <c r="C363" s="30"/>
       <c r="D363" s="30"/>
-      <c r="E363" s="36"/>
+      <c r="E363" s="31"/>
       <c r="F363" s="36"/>
       <c r="G363" s="30"/>
       <c r="H363" s="30"/>
@@ -6483,7 +5922,7 @@
       <c r="B364" s="30"/>
       <c r="C364" s="30"/>
       <c r="D364" s="30"/>
-      <c r="E364" s="36"/>
+      <c r="E364" s="31"/>
       <c r="F364" s="36"/>
       <c r="G364" s="30"/>
       <c r="H364" s="30"/>
@@ -6494,7 +5933,7 @@
       <c r="B365" s="30"/>
       <c r="C365" s="30"/>
       <c r="D365" s="30"/>
-      <c r="E365" s="36"/>
+      <c r="E365" s="31"/>
       <c r="F365" s="36"/>
       <c r="G365" s="30"/>
       <c r="H365" s="30"/>
@@ -6505,7 +5944,7 @@
       <c r="B366" s="30"/>
       <c r="C366" s="30"/>
       <c r="D366" s="30"/>
-      <c r="E366" s="36"/>
+      <c r="E366" s="31"/>
       <c r="F366" s="36"/>
       <c r="G366" s="30"/>
       <c r="H366" s="30"/>
@@ -6516,7 +5955,7 @@
       <c r="B367" s="30"/>
       <c r="C367" s="30"/>
       <c r="D367" s="30"/>
-      <c r="E367" s="36"/>
+      <c r="E367" s="31"/>
       <c r="F367" s="36"/>
       <c r="G367" s="30"/>
       <c r="H367" s="30"/>
@@ -6527,7 +5966,7 @@
       <c r="B368" s="30"/>
       <c r="C368" s="30"/>
       <c r="D368" s="30"/>
-      <c r="E368" s="36"/>
+      <c r="E368" s="31"/>
       <c r="F368" s="36"/>
       <c r="G368" s="30"/>
       <c r="H368" s="30"/>
@@ -6538,7 +5977,7 @@
       <c r="B369" s="30"/>
       <c r="C369" s="30"/>
       <c r="D369" s="30"/>
-      <c r="E369" s="36"/>
+      <c r="E369" s="31"/>
       <c r="F369" s="36"/>
       <c r="G369" s="30"/>
       <c r="H369" s="30"/>
@@ -6549,7 +5988,7 @@
       <c r="B370" s="30"/>
       <c r="C370" s="30"/>
       <c r="D370" s="30"/>
-      <c r="E370" s="36"/>
+      <c r="E370" s="31"/>
       <c r="F370" s="36"/>
       <c r="G370" s="30"/>
       <c r="H370" s="30"/>
@@ -6560,7 +5999,7 @@
       <c r="B371" s="30"/>
       <c r="C371" s="30"/>
       <c r="D371" s="30"/>
-      <c r="E371" s="36"/>
+      <c r="E371" s="31"/>
       <c r="F371" s="36"/>
       <c r="G371" s="30"/>
       <c r="H371" s="30"/>
@@ -6571,7 +6010,7 @@
       <c r="B372" s="30"/>
       <c r="C372" s="30"/>
       <c r="D372" s="30"/>
-      <c r="E372" s="36"/>
+      <c r="E372" s="31"/>
       <c r="F372" s="36"/>
       <c r="G372" s="30"/>
       <c r="H372" s="30"/>
@@ -6582,7 +6021,7 @@
       <c r="B373" s="30"/>
       <c r="C373" s="30"/>
       <c r="D373" s="30"/>
-      <c r="E373" s="36"/>
+      <c r="E373" s="31"/>
       <c r="F373" s="36"/>
       <c r="G373" s="30"/>
       <c r="H373" s="30"/>
@@ -6593,7 +6032,7 @@
       <c r="B374" s="30"/>
       <c r="C374" s="30"/>
       <c r="D374" s="30"/>
-      <c r="E374" s="36"/>
+      <c r="E374" s="31"/>
       <c r="F374" s="36"/>
       <c r="G374" s="30"/>
       <c r="H374" s="30"/>
@@ -6604,7 +6043,7 @@
       <c r="B375" s="30"/>
       <c r="C375" s="30"/>
       <c r="D375" s="30"/>
-      <c r="E375" s="36"/>
+      <c r="E375" s="31"/>
       <c r="F375" s="36"/>
       <c r="G375" s="30"/>
       <c r="H375" s="30"/>
@@ -6615,7 +6054,7 @@
       <c r="B376" s="30"/>
       <c r="C376" s="30"/>
       <c r="D376" s="30"/>
-      <c r="E376" s="36"/>
+      <c r="E376" s="31"/>
       <c r="F376" s="36"/>
       <c r="G376" s="30"/>
       <c r="H376" s="30"/>
@@ -6626,7 +6065,7 @@
       <c r="B377" s="30"/>
       <c r="C377" s="30"/>
       <c r="D377" s="30"/>
-      <c r="E377" s="36"/>
+      <c r="E377" s="31"/>
       <c r="F377" s="36"/>
       <c r="G377" s="30"/>
       <c r="H377" s="30"/>
@@ -6637,7 +6076,7 @@
       <c r="B378" s="30"/>
       <c r="C378" s="30"/>
       <c r="D378" s="30"/>
-      <c r="E378" s="36"/>
+      <c r="E378" s="31"/>
       <c r="F378" s="36"/>
       <c r="G378" s="30"/>
       <c r="H378" s="30"/>
@@ -6648,7 +6087,7 @@
       <c r="B379" s="30"/>
       <c r="C379" s="30"/>
       <c r="D379" s="30"/>
-      <c r="E379" s="36"/>
+      <c r="E379" s="31"/>
       <c r="F379" s="36"/>
       <c r="G379" s="30"/>
       <c r="H379" s="30"/>
@@ -6659,7 +6098,7 @@
       <c r="B380" s="30"/>
       <c r="C380" s="30"/>
       <c r="D380" s="30"/>
-      <c r="E380" s="36"/>
+      <c r="E380" s="31"/>
       <c r="F380" s="36"/>
       <c r="G380" s="30"/>
       <c r="H380" s="30"/>
@@ -6670,7 +6109,7 @@
       <c r="B381" s="30"/>
       <c r="C381" s="30"/>
       <c r="D381" s="30"/>
-      <c r="E381" s="36"/>
+      <c r="E381" s="31"/>
       <c r="F381" s="36"/>
       <c r="G381" s="30"/>
       <c r="H381" s="30"/>
@@ -6681,7 +6120,7 @@
       <c r="B382" s="30"/>
       <c r="C382" s="30"/>
       <c r="D382" s="30"/>
-      <c r="E382" s="36"/>
+      <c r="E382" s="31"/>
       <c r="F382" s="36"/>
       <c r="G382" s="30"/>
       <c r="H382" s="30"/>
@@ -6692,7 +6131,7 @@
       <c r="B383" s="30"/>
       <c r="C383" s="30"/>
       <c r="D383" s="30"/>
-      <c r="E383" s="36"/>
+      <c r="E383" s="31"/>
       <c r="F383" s="36"/>
       <c r="G383" s="30"/>
       <c r="H383" s="30"/>
@@ -6703,7 +6142,7 @@
       <c r="B384" s="30"/>
       <c r="C384" s="30"/>
       <c r="D384" s="30"/>
-      <c r="E384" s="36"/>
+      <c r="E384" s="31"/>
       <c r="F384" s="36"/>
       <c r="G384" s="30"/>
       <c r="H384" s="30"/>
@@ -6714,7 +6153,7 @@
       <c r="B385" s="30"/>
       <c r="C385" s="30"/>
       <c r="D385" s="30"/>
-      <c r="E385" s="36"/>
+      <c r="E385" s="31"/>
       <c r="F385" s="36"/>
       <c r="G385" s="30"/>
       <c r="H385" s="30"/>
@@ -6725,7 +6164,7 @@
       <c r="B386" s="30"/>
       <c r="C386" s="30"/>
       <c r="D386" s="30"/>
-      <c r="E386" s="36"/>
+      <c r="E386" s="31"/>
       <c r="F386" s="36"/>
       <c r="G386" s="30"/>
       <c r="H386" s="30"/>
@@ -6736,7 +6175,7 @@
       <c r="B387" s="30"/>
       <c r="C387" s="30"/>
       <c r="D387" s="30"/>
-      <c r="E387" s="36"/>
+      <c r="E387" s="31"/>
       <c r="F387" s="36"/>
       <c r="G387" s="30"/>
       <c r="H387" s="30"/>
@@ -6747,7 +6186,7 @@
       <c r="B388" s="30"/>
       <c r="C388" s="30"/>
       <c r="D388" s="30"/>
-      <c r="E388" s="36"/>
+      <c r="E388" s="31"/>
       <c r="F388" s="36"/>
       <c r="G388" s="30"/>
       <c r="H388" s="30"/>
@@ -6758,7 +6197,7 @@
       <c r="B389" s="30"/>
       <c r="C389" s="30"/>
       <c r="D389" s="30"/>
-      <c r="E389" s="36"/>
+      <c r="E389" s="31"/>
       <c r="F389" s="36"/>
       <c r="G389" s="30"/>
       <c r="H389" s="30"/>
@@ -6769,7 +6208,7 @@
       <c r="B390" s="30"/>
       <c r="C390" s="30"/>
       <c r="D390" s="30"/>
-      <c r="E390" s="36"/>
+      <c r="E390" s="31"/>
       <c r="F390" s="36"/>
       <c r="G390" s="30"/>
       <c r="H390" s="30"/>
@@ -6780,7 +6219,7 @@
       <c r="B391" s="30"/>
       <c r="C391" s="30"/>
       <c r="D391" s="30"/>
-      <c r="E391" s="36"/>
+      <c r="E391" s="31"/>
       <c r="F391" s="36"/>
       <c r="G391" s="30"/>
       <c r="H391" s="30"/>
@@ -6791,7 +6230,7 @@
       <c r="B392" s="30"/>
       <c r="C392" s="30"/>
       <c r="D392" s="30"/>
-      <c r="E392" s="36"/>
+      <c r="E392" s="31"/>
       <c r="F392" s="36"/>
       <c r="G392" s="30"/>
       <c r="H392" s="30"/>
@@ -6802,7 +6241,7 @@
       <c r="B393" s="30"/>
       <c r="C393" s="30"/>
       <c r="D393" s="30"/>
-      <c r="E393" s="36"/>
+      <c r="E393" s="31"/>
       <c r="F393" s="36"/>
       <c r="G393" s="30"/>
       <c r="H393" s="30"/>
@@ -6813,7 +6252,7 @@
       <c r="B394" s="30"/>
       <c r="C394" s="30"/>
       <c r="D394" s="30"/>
-      <c r="E394" s="36"/>
+      <c r="E394" s="31"/>
       <c r="F394" s="36"/>
       <c r="G394" s="30"/>
       <c r="H394" s="30"/>
@@ -6824,7 +6263,7 @@
       <c r="B395" s="30"/>
       <c r="C395" s="30"/>
       <c r="D395" s="30"/>
-      <c r="E395" s="36"/>
+      <c r="E395" s="31"/>
       <c r="F395" s="36"/>
       <c r="G395" s="30"/>
       <c r="H395" s="30"/>
@@ -6835,7 +6274,7 @@
       <c r="B396" s="30"/>
       <c r="C396" s="30"/>
       <c r="D396" s="30"/>
-      <c r="E396" s="36"/>
+      <c r="E396" s="31"/>
       <c r="F396" s="36"/>
       <c r="G396" s="30"/>
       <c r="H396" s="30"/>
@@ -6846,7 +6285,7 @@
       <c r="B397" s="30"/>
       <c r="C397" s="30"/>
       <c r="D397" s="30"/>
-      <c r="E397" s="36"/>
+      <c r="E397" s="31"/>
       <c r="F397" s="36"/>
       <c r="G397" s="30"/>
       <c r="H397" s="30"/>
@@ -6857,7 +6296,7 @@
       <c r="B398" s="30"/>
       <c r="C398" s="30"/>
       <c r="D398" s="30"/>
-      <c r="E398" s="36"/>
+      <c r="E398" s="31"/>
       <c r="F398" s="36"/>
       <c r="G398" s="30"/>
       <c r="H398" s="30"/>
@@ -6868,7 +6307,7 @@
       <c r="B399" s="30"/>
       <c r="C399" s="30"/>
       <c r="D399" s="30"/>
-      <c r="E399" s="36"/>
+      <c r="E399" s="31"/>
       <c r="F399" s="36"/>
       <c r="G399" s="30"/>
       <c r="H399" s="30"/>
@@ -6879,7 +6318,7 @@
       <c r="B400" s="30"/>
       <c r="C400" s="30"/>
       <c r="D400" s="30"/>
-      <c r="E400" s="36"/>
+      <c r="E400" s="31"/>
       <c r="F400" s="36"/>
       <c r="G400" s="30"/>
       <c r="H400" s="30"/>
@@ -6907,18 +6346,18 @@
     <sortCondition ref="A6:F6"/>
   </sortState>
   <conditionalFormatting sqref="F7:F400">
-    <cfRule type="cellIs" dxfId="37" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="lessThan">
       <formula>NOW()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:G400">
-    <cfRule type="containsText" dxfId="36" priority="8" operator="containsText" text="In Arbeit">
+    <cfRule type="containsText" dxfId="5" priority="8" operator="containsText" text="In Arbeit">
       <formula>NOT(ISERROR(SEARCH("In Arbeit",G7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="7" operator="containsText" text="Offen">
+    <cfRule type="containsText" dxfId="4" priority="7" operator="containsText" text="Offen">
       <formula>NOT(ISERROR(SEARCH("Offen",G7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="6" operator="containsText" text="Erledigt">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Erledigt">
       <formula>NOT(ISERROR(SEARCH("Erledigt",G7)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6950,7 +6389,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16"/>
@@ -11774,15 +11213,15 @@
   <autoFilter ref="A6:J143" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <dataConsolidate/>
   <conditionalFormatting sqref="H43:H143 H7:H400">
-    <cfRule type="containsText" dxfId="5" priority="16" operator="containsText" text="Mittel">
+    <cfRule type="containsText" dxfId="2" priority="16" operator="containsText" text="Mittel">
       <formula>NOT(ISERROR(SEARCH("Mittel",H7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:H400">
-    <cfRule type="containsText" dxfId="4" priority="18" operator="containsText" text="Hoch">
+    <cfRule type="containsText" dxfId="1" priority="18" operator="containsText" text="Hoch">
       <formula>NOT(ISERROR(SEARCH("Hoch",H7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="17" operator="containsText" text="Gering">
+    <cfRule type="containsText" dxfId="0" priority="17" operator="containsText" text="Gering">
       <formula>NOT(ISERROR(SEARCH("Gering",H7)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11819,6 +11258,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Documenttype xmlns="F56B8473-376F-4348-9824-7D53304FEF34">Others</Documenttype>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -11827,7 +11274,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010002EBCB0075CDE848B9F1103A71226B95" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31da03af10aa6052cd3ee1f9464c6d23">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="F56B8473-376F-4348-9824-7D53304FEF34" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f1d4c1356f931c1151e9b07ac54607de" ns2:_="">
     <xsd:import namespace="F56B8473-376F-4348-9824-7D53304FEF34"/>
@@ -11962,15 +11409,23 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Documenttype xmlns="F56B8473-376F-4348-9824-7D53304FEF34">Others</Documenttype>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50A734F2-ABF0-4EAB-8144-986899B49A09}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="F56B8473-376F-4348-9824-7D53304FEF34"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{305E179E-B965-420A-9666-EB4FCA089A80}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -11978,7 +11433,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B7583A5-096C-40FC-AE3B-CFC4E2E0AEEC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11994,20 +11449,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50A734F2-ABF0-4EAB-8144-986899B49A09}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="F56B8473-376F-4348-9824-7D53304FEF34"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>